<commit_message>
Show Subjects and Hide Programming Languages for teach
</commit_message>
<xml_diff>
--- a/resources/excel/resources-teach.xlsx
+++ b/resources/excel/resources-teach.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="42620" windowHeight="26920" tabRatio="500"/>
+    <workbookView xWindow="25600" yWindow="0" windowWidth="25600" windowHeight="26740" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="20190114-Teach-Database" sheetId="1" r:id="rId1"/>
@@ -526,9 +526,6 @@
     <t>https://i.ytimg.com/vi/Cv6f-2Wlsxg/maxresdefault.jpg</t>
   </si>
   <si>
-    <t>Foreign Languages; Language and Literature;Mathematics; Natural science; History; Music; Computer Science; Art</t>
-  </si>
-  <si>
     <t xml:space="preserve">Primary school (5-12); Lower secondary school (12-16); </t>
   </si>
   <si>
@@ -593,9 +590,6 @@
   </si>
   <si>
     <t>http://www.skolskiportal.edu.me/PublishingImages/skolski-portal3.png</t>
-  </si>
-  <si>
-    <t>Computer science; Programming; Coding; Maths;  Other;</t>
   </si>
   <si>
     <t>Kodu GameLab Community</t>
@@ -1072,9 +1066,6 @@
     <t xml:space="preserve">Lesson plan; Website; Game; </t>
   </si>
   <si>
-    <t>Art; Biology; Chemistry; Computer science; Culture; Economics; Foreign Languages; Geography; Geology; History; Language and Literature; Mathematics; Natural sciences; Physical Education; Physics; Programming; Coding; Other Needs; Other</t>
-  </si>
-  <si>
     <t>Pre-primary education; Primary school (5-12); Lower secondary school (12-16); Upper secondary school (16-18); Higher education; Other; Other;</t>
   </si>
   <si>
@@ -1094,6 +1085,15 @@
   </si>
   <si>
     <t>Scratch Jr by MIT</t>
+  </si>
+  <si>
+    <t>Computer science; Programming; Coding; Mathematics;  Other;</t>
+  </si>
+  <si>
+    <t>Foreign Languages; Language and Literature;Mathematics; Natural sciences; History; Music; Computer Science; Art</t>
+  </si>
+  <si>
+    <t>Art; Biology; Chemistry; Computer science; Culture; Economics; Foreign Languages; Geography; Geology; History; Language and Literature; Mathematics; Natural sciences; Physical Education; Physics; Programming; Coding; Other; Other</t>
   </si>
 </sst>
 </file>
@@ -1907,8 +1907,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" topLeftCell="G2" workbookViewId="0">
+      <selection activeCell="I23" sqref="I23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0"/>
@@ -1921,7 +1921,7 @@
     <col min="6" max="6" width="34.6640625" customWidth="1"/>
     <col min="7" max="7" width="34.5" customWidth="1"/>
     <col min="8" max="8" width="64.33203125" customWidth="1"/>
-    <col min="9" max="9" width="22.6640625" customWidth="1"/>
+    <col min="9" max="9" width="61.6640625" customWidth="1"/>
     <col min="10" max="10" width="54" customWidth="1"/>
     <col min="11" max="26" width="8.6640625" customWidth="1"/>
   </cols>
@@ -1976,7 +1976,7 @@
     </row>
     <row r="2" spans="1:26" ht="14">
       <c r="A2" s="5" t="s">
-        <v>333</v>
+        <v>330</v>
       </c>
       <c r="B2" s="7" t="s">
         <v>17</v>
@@ -1999,8 +1999,8 @@
       <c r="H2" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="I2" s="8" t="s">
-        <v>327</v>
+      <c r="I2" s="36" t="s">
+        <v>334</v>
       </c>
       <c r="J2" s="11" t="s">
         <v>35</v>
@@ -2024,7 +2024,7 @@
     </row>
     <row r="3" spans="1:26" ht="14">
       <c r="A3" s="5" t="s">
-        <v>334</v>
+        <v>331</v>
       </c>
       <c r="B3" s="7" t="s">
         <v>43</v>
@@ -2048,7 +2048,7 @@
         <v>59</v>
       </c>
       <c r="I3" s="8" t="s">
-        <v>327</v>
+        <v>334</v>
       </c>
       <c r="J3" s="11" t="s">
         <v>12</v>
@@ -2087,7 +2087,7 @@
         <v>16</v>
       </c>
       <c r="F4" s="8" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="G4" s="5" t="s">
         <v>72</v>
@@ -2144,7 +2144,7 @@
         <v>89</v>
       </c>
       <c r="I5" s="8" t="s">
-        <v>327</v>
+        <v>334</v>
       </c>
       <c r="J5" s="11" t="s">
         <v>94</v>
@@ -2177,7 +2177,7 @@
         <v>97</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="E6" s="8" t="s">
         <v>16</v>
@@ -2337,7 +2337,7 @@
       </c>
       <c r="I9" s="8"/>
       <c r="J9" s="11" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="K9" s="12"/>
       <c r="L9" s="12"/>
@@ -2364,7 +2364,7 @@
         <v>124</v>
       </c>
       <c r="C10" s="8" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="D10" s="8" t="s">
         <v>22</v>
@@ -2426,7 +2426,7 @@
       </c>
       <c r="H11" s="18"/>
       <c r="I11" s="8" t="s">
-        <v>327</v>
+        <v>334</v>
       </c>
       <c r="J11" s="11" t="s">
         <v>102</v>
@@ -2462,7 +2462,7 @@
         <v>22</v>
       </c>
       <c r="E12" s="8" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="F12" s="8" t="s">
         <v>126</v>
@@ -2552,7 +2552,7 @@
         <v>150</v>
       </c>
       <c r="C14" s="8" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="D14" s="8" t="s">
         <v>22</v>
@@ -2646,7 +2646,7 @@
         <v>163</v>
       </c>
       <c r="C16" s="8" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="D16" s="8" t="s">
         <v>22</v>
@@ -2664,10 +2664,10 @@
         <v>166</v>
       </c>
       <c r="I16" s="8" t="s">
+        <v>333</v>
+      </c>
+      <c r="J16" s="11" t="s">
         <v>167</v>
-      </c>
-      <c r="J16" s="11" t="s">
-        <v>168</v>
       </c>
       <c r="K16" s="12"/>
       <c r="L16" s="12"/>
@@ -2688,10 +2688,10 @@
     </row>
     <row r="17" spans="1:26" ht="14">
       <c r="A17" s="5" t="s">
+        <v>168</v>
+      </c>
+      <c r="B17" s="7" t="s">
         <v>169</v>
-      </c>
-      <c r="B17" s="7" t="s">
-        <v>170</v>
       </c>
       <c r="C17" s="8" t="s">
         <v>157</v>
@@ -2700,22 +2700,22 @@
         <v>22</v>
       </c>
       <c r="E17" s="8" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="F17" s="8" t="s">
         <v>126</v>
       </c>
       <c r="G17" s="5" t="s">
+        <v>171</v>
+      </c>
+      <c r="H17" s="5" t="s">
         <v>172</v>
       </c>
-      <c r="H17" s="5" t="s">
+      <c r="I17" s="8" t="s">
         <v>173</v>
       </c>
-      <c r="I17" s="8" t="s">
+      <c r="J17" s="11" t="s">
         <v>174</v>
-      </c>
-      <c r="J17" s="11" t="s">
-        <v>175</v>
       </c>
       <c r="K17" s="12"/>
       <c r="L17" s="12"/>
@@ -2736,10 +2736,10 @@
     </row>
     <row r="18" spans="1:26" ht="14">
       <c r="A18" s="5" t="s">
+        <v>175</v>
+      </c>
+      <c r="B18" s="7" t="s">
         <v>176</v>
-      </c>
-      <c r="B18" s="7" t="s">
-        <v>177</v>
       </c>
       <c r="C18" s="8" t="s">
         <v>157</v>
@@ -2748,20 +2748,20 @@
         <v>22</v>
       </c>
       <c r="E18" s="8" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="F18" s="8" t="s">
         <v>126</v>
       </c>
       <c r="G18" s="5" t="s">
+        <v>178</v>
+      </c>
+      <c r="H18" s="5" t="s">
         <v>179</v>
-      </c>
-      <c r="H18" s="5" t="s">
-        <v>180</v>
       </c>
       <c r="I18" s="8"/>
       <c r="J18" s="11" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="K18" s="12"/>
       <c r="L18" s="12"/>
@@ -2782,34 +2782,34 @@
     </row>
     <row r="19" spans="1:26" ht="42">
       <c r="A19" s="5" t="s">
+        <v>181</v>
+      </c>
+      <c r="B19" s="23" t="s">
         <v>182</v>
       </c>
-      <c r="B19" s="23" t="s">
+      <c r="C19" s="8" t="s">
         <v>183</v>
       </c>
-      <c r="C19" s="8" t="s">
+      <c r="D19" s="8" t="s">
         <v>184</v>
       </c>
-      <c r="D19" s="8" t="s">
+      <c r="E19" s="8" t="s">
         <v>185</v>
       </c>
-      <c r="E19" s="8" t="s">
+      <c r="F19" s="8" t="s">
         <v>186</v>
       </c>
-      <c r="F19" s="8" t="s">
+      <c r="G19" s="22" t="s">
         <v>187</v>
       </c>
-      <c r="G19" s="22" t="s">
+      <c r="H19" s="22" t="s">
         <v>188</v>
       </c>
-      <c r="H19" s="22" t="s">
-        <v>189</v>
-      </c>
       <c r="I19" s="8" t="s">
-        <v>190</v>
+        <v>332</v>
       </c>
       <c r="J19" s="11" t="s">
-        <v>328</v>
+        <v>325</v>
       </c>
       <c r="K19" s="12"/>
       <c r="L19" s="12"/>
@@ -2830,31 +2830,31 @@
     </row>
     <row r="20" spans="1:26" ht="28">
       <c r="A20" s="5" t="s">
+        <v>189</v>
+      </c>
+      <c r="B20" s="7" t="s">
+        <v>190</v>
+      </c>
+      <c r="C20" s="8" t="s">
         <v>191</v>
       </c>
-      <c r="B20" s="7" t="s">
-        <v>192</v>
-      </c>
-      <c r="C20" s="8" t="s">
-        <v>193</v>
-      </c>
       <c r="D20" s="8" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="E20" s="8" t="s">
         <v>23</v>
       </c>
       <c r="F20" s="8" t="s">
+        <v>192</v>
+      </c>
+      <c r="G20" s="5" t="s">
+        <v>193</v>
+      </c>
+      <c r="H20" s="5" t="s">
         <v>194</v>
       </c>
-      <c r="G20" s="5" t="s">
+      <c r="I20" s="8" t="s">
         <v>195</v>
-      </c>
-      <c r="H20" s="5" t="s">
-        <v>196</v>
-      </c>
-      <c r="I20" s="8" t="s">
-        <v>197</v>
       </c>
       <c r="J20" s="11" t="s">
         <v>94</v>
@@ -2878,29 +2878,29 @@
     </row>
     <row r="21" spans="1:26" ht="15.75" customHeight="1">
       <c r="A21" s="5" t="s">
+        <v>196</v>
+      </c>
+      <c r="B21" s="7" t="s">
+        <v>197</v>
+      </c>
+      <c r="C21" s="8" t="s">
         <v>198</v>
       </c>
-      <c r="B21" s="7" t="s">
+      <c r="D21" s="8" t="s">
         <v>199</v>
       </c>
-      <c r="C21" s="8" t="s">
+      <c r="E21" s="8" t="s">
         <v>200</v>
       </c>
-      <c r="D21" s="8" t="s">
+      <c r="F21" s="24" t="s">
         <v>201</v>
       </c>
-      <c r="E21" s="8" t="s">
+      <c r="G21" s="5" t="s">
         <v>202</v>
-      </c>
-      <c r="F21" s="24" t="s">
-        <v>203</v>
-      </c>
-      <c r="G21" s="5" t="s">
-        <v>204</v>
       </c>
       <c r="H21" s="25"/>
       <c r="I21" s="8" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="J21" s="11" t="s">
         <v>35</v>
@@ -2924,34 +2924,34 @@
     </row>
     <row r="22" spans="1:26" ht="15.75" customHeight="1">
       <c r="A22" s="5" t="s">
+        <v>204</v>
+      </c>
+      <c r="B22" s="7" t="s">
+        <v>205</v>
+      </c>
+      <c r="C22" s="8" t="s">
         <v>206</v>
       </c>
-      <c r="B22" s="7" t="s">
+      <c r="D22" s="8" t="s">
+        <v>184</v>
+      </c>
+      <c r="E22" s="8" t="s">
+        <v>200</v>
+      </c>
+      <c r="F22" s="8" t="s">
+        <v>317</v>
+      </c>
+      <c r="G22" s="5" t="s">
         <v>207</v>
       </c>
-      <c r="C22" s="8" t="s">
+      <c r="H22" s="5" t="s">
         <v>208</v>
       </c>
-      <c r="D22" s="8" t="s">
-        <v>185</v>
-      </c>
-      <c r="E22" s="8" t="s">
-        <v>202</v>
-      </c>
-      <c r="F22" s="8" t="s">
-        <v>319</v>
-      </c>
-      <c r="G22" s="5" t="s">
+      <c r="I22" s="8" t="s">
         <v>209</v>
       </c>
-      <c r="H22" s="5" t="s">
+      <c r="J22" s="11" t="s">
         <v>210</v>
-      </c>
-      <c r="I22" s="8" t="s">
-        <v>211</v>
-      </c>
-      <c r="J22" s="11" t="s">
-        <v>212</v>
       </c>
       <c r="K22" s="12"/>
       <c r="L22" s="12"/>
@@ -2972,32 +2972,32 @@
     </row>
     <row r="23" spans="1:26" ht="15.75" customHeight="1">
       <c r="A23" s="5" t="s">
+        <v>211</v>
+      </c>
+      <c r="B23" s="23" t="s">
+        <v>212</v>
+      </c>
+      <c r="C23" s="8" t="s">
         <v>213</v>
       </c>
-      <c r="B23" s="23" t="s">
+      <c r="D23" s="7" t="s">
+        <v>184</v>
+      </c>
+      <c r="E23" s="8" t="s">
         <v>214</v>
       </c>
-      <c r="C23" s="8" t="s">
+      <c r="F23" s="8" t="s">
         <v>215</v>
       </c>
-      <c r="D23" s="7" t="s">
-        <v>185</v>
-      </c>
-      <c r="E23" s="8" t="s">
+      <c r="G23" s="22" t="s">
         <v>216</v>
-      </c>
-      <c r="F23" s="8" t="s">
-        <v>217</v>
-      </c>
-      <c r="G23" s="22" t="s">
-        <v>218</v>
       </c>
       <c r="H23" s="26"/>
       <c r="I23" s="8" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="J23" s="20" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="K23" s="12"/>
       <c r="L23" s="12"/>
@@ -3018,34 +3018,34 @@
     </row>
     <row r="24" spans="1:26" ht="15.75" customHeight="1">
       <c r="A24" s="5" t="s">
+        <v>219</v>
+      </c>
+      <c r="B24" s="23" t="s">
+        <v>220</v>
+      </c>
+      <c r="C24" s="8" t="s">
         <v>221</v>
       </c>
-      <c r="B24" s="23" t="s">
+      <c r="D24" s="7" t="s">
+        <v>184</v>
+      </c>
+      <c r="E24" s="8" t="s">
+        <v>200</v>
+      </c>
+      <c r="F24" s="8" t="s">
         <v>222</v>
       </c>
-      <c r="C24" s="8" t="s">
+      <c r="G24" s="22" t="s">
         <v>223</v>
       </c>
-      <c r="D24" s="7" t="s">
-        <v>185</v>
-      </c>
-      <c r="E24" s="8" t="s">
-        <v>202</v>
-      </c>
-      <c r="F24" s="8" t="s">
+      <c r="H24" s="22" t="s">
         <v>224</v>
       </c>
-      <c r="G24" s="22" t="s">
-        <v>225</v>
-      </c>
-      <c r="H24" s="22" t="s">
-        <v>226</v>
-      </c>
       <c r="I24" s="8" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="J24" s="20" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="K24" s="12"/>
       <c r="L24" s="12"/>
@@ -3066,34 +3066,34 @@
     </row>
     <row r="25" spans="1:26" ht="15.75" customHeight="1">
       <c r="A25" s="5" t="s">
+        <v>225</v>
+      </c>
+      <c r="B25" s="23" t="s">
+        <v>226</v>
+      </c>
+      <c r="C25" s="8" t="s">
+        <v>206</v>
+      </c>
+      <c r="D25" s="7" t="s">
         <v>227</v>
       </c>
-      <c r="B25" s="23" t="s">
+      <c r="E25" s="8" t="s">
+        <v>200</v>
+      </c>
+      <c r="F25" s="8" t="s">
+        <v>222</v>
+      </c>
+      <c r="G25" s="22" t="s">
         <v>228</v>
       </c>
-      <c r="C25" s="8" t="s">
-        <v>208</v>
-      </c>
-      <c r="D25" s="7" t="s">
+      <c r="H25" s="22" t="s">
         <v>229</v>
       </c>
-      <c r="E25" s="8" t="s">
-        <v>202</v>
-      </c>
-      <c r="F25" s="8" t="s">
-        <v>224</v>
-      </c>
-      <c r="G25" s="22" t="s">
+      <c r="I25" s="8" t="s">
+        <v>217</v>
+      </c>
+      <c r="J25" s="20" t="s">
         <v>230</v>
-      </c>
-      <c r="H25" s="22" t="s">
-        <v>231</v>
-      </c>
-      <c r="I25" s="8" t="s">
-        <v>219</v>
-      </c>
-      <c r="J25" s="20" t="s">
-        <v>232</v>
       </c>
       <c r="K25" s="12"/>
       <c r="L25" s="12"/>
@@ -3114,32 +3114,32 @@
     </row>
     <row r="26" spans="1:26" ht="15.75" customHeight="1">
       <c r="A26" s="17" t="s">
+        <v>231</v>
+      </c>
+      <c r="B26" s="23" t="s">
+        <v>232</v>
+      </c>
+      <c r="C26" s="8" t="s">
         <v>233</v>
       </c>
-      <c r="B26" s="23" t="s">
+      <c r="D26" s="8" t="s">
+        <v>184</v>
+      </c>
+      <c r="E26" s="8" t="s">
+        <v>200</v>
+      </c>
+      <c r="F26" s="8" t="s">
         <v>234</v>
       </c>
-      <c r="C26" s="8" t="s">
+      <c r="G26" s="22" t="s">
         <v>235</v>
-      </c>
-      <c r="D26" s="8" t="s">
-        <v>185</v>
-      </c>
-      <c r="E26" s="8" t="s">
-        <v>202</v>
-      </c>
-      <c r="F26" s="8" t="s">
-        <v>236</v>
-      </c>
-      <c r="G26" s="22" t="s">
-        <v>237</v>
       </c>
       <c r="H26" s="27"/>
       <c r="I26" s="8" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="J26" s="20" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="K26" s="12"/>
       <c r="L26" s="12"/>
@@ -3160,31 +3160,31 @@
     </row>
     <row r="27" spans="1:26" ht="15.75" customHeight="1">
       <c r="A27" s="5" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="B27" s="23" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="C27" s="8" t="s">
         <v>132</v>
       </c>
       <c r="D27" s="8" t="s">
+        <v>239</v>
+      </c>
+      <c r="E27" s="8" t="s">
+        <v>200</v>
+      </c>
+      <c r="F27" s="8" t="s">
+        <v>240</v>
+      </c>
+      <c r="G27" s="22" t="s">
         <v>241</v>
       </c>
-      <c r="E27" s="8" t="s">
-        <v>202</v>
-      </c>
-      <c r="F27" s="8" t="s">
+      <c r="H27" s="22" t="s">
         <v>242</v>
       </c>
-      <c r="G27" s="22" t="s">
+      <c r="I27" s="8" t="s">
         <v>243</v>
-      </c>
-      <c r="H27" s="22" t="s">
-        <v>244</v>
-      </c>
-      <c r="I27" s="8" t="s">
-        <v>245</v>
       </c>
       <c r="J27" s="11" t="s">
         <v>78</v>
@@ -3208,34 +3208,34 @@
     </row>
     <row r="28" spans="1:26" ht="15.75" customHeight="1">
       <c r="A28" s="5" t="s">
+        <v>244</v>
+      </c>
+      <c r="B28" s="23" t="s">
+        <v>245</v>
+      </c>
+      <c r="C28" s="36" t="s">
+        <v>321</v>
+      </c>
+      <c r="D28" s="16" t="s">
         <v>246</v>
       </c>
-      <c r="B28" s="23" t="s">
+      <c r="E28" s="8" t="s">
+        <v>200</v>
+      </c>
+      <c r="F28" s="8" t="s">
+        <v>240</v>
+      </c>
+      <c r="G28" s="22" t="s">
         <v>247</v>
       </c>
-      <c r="C28" s="36" t="s">
-        <v>323</v>
-      </c>
-      <c r="D28" s="16" t="s">
+      <c r="H28" s="22" t="s">
         <v>248</v>
       </c>
-      <c r="E28" s="8" t="s">
-        <v>202</v>
-      </c>
-      <c r="F28" s="8" t="s">
-        <v>242</v>
-      </c>
-      <c r="G28" s="22" t="s">
+      <c r="I28" s="8" t="s">
         <v>249</v>
       </c>
-      <c r="H28" s="22" t="s">
-        <v>250</v>
-      </c>
-      <c r="I28" s="8" t="s">
-        <v>251</v>
-      </c>
       <c r="J28" s="11" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="K28" s="12"/>
       <c r="L28" s="12"/>
@@ -3256,32 +3256,32 @@
     </row>
     <row r="29" spans="1:26" ht="15.75" customHeight="1">
       <c r="A29" s="5" t="s">
+        <v>250</v>
+      </c>
+      <c r="B29" s="23" t="s">
+        <v>251</v>
+      </c>
+      <c r="C29" s="28" t="s">
         <v>252</v>
       </c>
-      <c r="B29" s="23" t="s">
+      <c r="D29" s="8" t="s">
         <v>253</v>
       </c>
-      <c r="C29" s="28" t="s">
+      <c r="E29" s="29" t="s">
         <v>254</v>
       </c>
-      <c r="D29" s="8" t="s">
+      <c r="F29" s="8" t="s">
         <v>255</v>
       </c>
-      <c r="E29" s="29" t="s">
+      <c r="G29" s="22" t="s">
         <v>256</v>
-      </c>
-      <c r="F29" s="8" t="s">
-        <v>257</v>
-      </c>
-      <c r="G29" s="22" t="s">
-        <v>258</v>
       </c>
       <c r="H29" s="30"/>
       <c r="I29" s="8" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="J29" s="11" t="s">
-        <v>330</v>
+        <v>327</v>
       </c>
       <c r="K29" s="12"/>
       <c r="L29" s="12"/>
@@ -3302,31 +3302,31 @@
     </row>
     <row r="30" spans="1:26" ht="15.75" customHeight="1">
       <c r="A30" s="5" t="s">
+        <v>258</v>
+      </c>
+      <c r="B30" s="7" t="s">
+        <v>259</v>
+      </c>
+      <c r="C30" s="8" t="s">
         <v>260</v>
       </c>
-      <c r="B30" s="7" t="s">
+      <c r="D30" s="31" t="s">
         <v>261</v>
       </c>
-      <c r="C30" s="8" t="s">
+      <c r="E30" s="8" t="s">
+        <v>200</v>
+      </c>
+      <c r="F30" s="8" t="s">
+        <v>240</v>
+      </c>
+      <c r="G30" s="5" t="s">
         <v>262</v>
       </c>
-      <c r="D30" s="31" t="s">
+      <c r="H30" s="5" t="s">
         <v>263</v>
       </c>
-      <c r="E30" s="8" t="s">
-        <v>202</v>
-      </c>
-      <c r="F30" s="8" t="s">
-        <v>242</v>
-      </c>
-      <c r="G30" s="5" t="s">
+      <c r="I30" s="8" t="s">
         <v>264</v>
-      </c>
-      <c r="H30" s="5" t="s">
-        <v>265</v>
-      </c>
-      <c r="I30" s="8" t="s">
-        <v>266</v>
       </c>
       <c r="J30" s="11" t="s">
         <v>94</v>
@@ -3350,31 +3350,31 @@
     </row>
     <row r="31" spans="1:26" ht="15.75" customHeight="1">
       <c r="A31" s="5" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="B31" s="7" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="C31" s="8" t="s">
         <v>157</v>
       </c>
       <c r="D31" s="8" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="E31" s="28" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="F31" s="8" t="s">
+        <v>267</v>
+      </c>
+      <c r="G31" s="5" t="s">
+        <v>268</v>
+      </c>
+      <c r="H31" s="5" t="s">
         <v>269</v>
       </c>
-      <c r="G31" s="5" t="s">
-        <v>270</v>
-      </c>
-      <c r="H31" s="5" t="s">
-        <v>271</v>
-      </c>
       <c r="I31" s="8" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="J31" s="11" t="s">
         <v>94</v>
@@ -3398,34 +3398,34 @@
     </row>
     <row r="32" spans="1:26" ht="15.75" customHeight="1">
       <c r="A32" s="5" t="s">
+        <v>270</v>
+      </c>
+      <c r="B32" s="7" t="s">
+        <v>271</v>
+      </c>
+      <c r="C32" s="8" t="s">
         <v>272</v>
       </c>
-      <c r="B32" s="7" t="s">
-        <v>273</v>
-      </c>
-      <c r="C32" s="8" t="s">
-        <v>274</v>
-      </c>
       <c r="D32" s="8" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="E32" s="8" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="F32" s="8" t="s">
         <v>126</v>
       </c>
       <c r="G32" s="5" t="s">
+        <v>273</v>
+      </c>
+      <c r="H32" s="5" t="s">
+        <v>274</v>
+      </c>
+      <c r="I32" s="8" t="s">
+        <v>257</v>
+      </c>
+      <c r="J32" s="11" t="s">
         <v>275</v>
-      </c>
-      <c r="H32" s="5" t="s">
-        <v>276</v>
-      </c>
-      <c r="I32" s="8" t="s">
-        <v>259</v>
-      </c>
-      <c r="J32" s="11" t="s">
-        <v>277</v>
       </c>
       <c r="K32" s="12"/>
       <c r="L32" s="12"/>
@@ -3446,34 +3446,34 @@
     </row>
     <row r="33" spans="1:26" ht="15.75" customHeight="1">
       <c r="A33" s="5" t="s">
+        <v>276</v>
+      </c>
+      <c r="B33" s="7" t="s">
+        <v>277</v>
+      </c>
+      <c r="C33" s="8" t="s">
         <v>278</v>
       </c>
-      <c r="B33" s="7" t="s">
+      <c r="D33" s="8" t="s">
         <v>279</v>
       </c>
-      <c r="C33" s="8" t="s">
-        <v>280</v>
-      </c>
-      <c r="D33" s="8" t="s">
-        <v>281</v>
-      </c>
       <c r="E33" s="8" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="F33" s="8" t="s">
         <v>126</v>
       </c>
       <c r="G33" s="5" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="H33" s="5" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="I33" s="8" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="J33" s="11" t="s">
-        <v>329</v>
+        <v>326</v>
       </c>
       <c r="K33" s="12"/>
       <c r="L33" s="12"/>
@@ -3494,34 +3494,34 @@
     </row>
     <row r="34" spans="1:26" ht="15.75" customHeight="1">
       <c r="A34" s="5" t="s">
+        <v>282</v>
+      </c>
+      <c r="B34" s="7" t="s">
+        <v>283</v>
+      </c>
+      <c r="C34" s="8" t="s">
         <v>284</v>
       </c>
-      <c r="B34" s="7" t="s">
+      <c r="D34" s="8" t="s">
+        <v>243</v>
+      </c>
+      <c r="E34" s="8" t="s">
         <v>285</v>
-      </c>
-      <c r="C34" s="8" t="s">
-        <v>286</v>
-      </c>
-      <c r="D34" s="8" t="s">
-        <v>245</v>
-      </c>
-      <c r="E34" s="8" t="s">
-        <v>287</v>
       </c>
       <c r="F34" s="8" t="s">
         <v>126</v>
       </c>
       <c r="G34" s="5" t="s">
+        <v>286</v>
+      </c>
+      <c r="H34" s="5" t="s">
+        <v>287</v>
+      </c>
+      <c r="I34" s="8" t="s">
         <v>288</v>
       </c>
-      <c r="H34" s="5" t="s">
+      <c r="J34" s="11" t="s">
         <v>289</v>
-      </c>
-      <c r="I34" s="8" t="s">
-        <v>290</v>
-      </c>
-      <c r="J34" s="11" t="s">
-        <v>291</v>
       </c>
       <c r="K34" s="12"/>
       <c r="L34" s="12"/>
@@ -3542,10 +3542,10 @@
     </row>
     <row r="35" spans="1:26" ht="15.75" customHeight="1">
       <c r="A35" s="5" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="B35" s="7" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="C35" s="8" t="s">
         <v>157</v>
@@ -3554,22 +3554,22 @@
         <v>22</v>
       </c>
       <c r="E35" s="8" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="F35" s="8" t="s">
         <v>126</v>
       </c>
       <c r="G35" s="5" t="s">
+        <v>292</v>
+      </c>
+      <c r="H35" s="5" t="s">
+        <v>293</v>
+      </c>
+      <c r="I35" s="8" t="s">
+        <v>257</v>
+      </c>
+      <c r="J35" s="11" t="s">
         <v>294</v>
-      </c>
-      <c r="H35" s="5" t="s">
-        <v>295</v>
-      </c>
-      <c r="I35" s="8" t="s">
-        <v>259</v>
-      </c>
-      <c r="J35" s="11" t="s">
-        <v>296</v>
       </c>
       <c r="K35" s="12"/>
       <c r="L35" s="12"/>
@@ -3590,31 +3590,31 @@
     </row>
     <row r="36" spans="1:26" ht="15.75" customHeight="1">
       <c r="A36" s="5" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="B36" s="23" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="C36" s="8" t="s">
         <v>132</v>
       </c>
       <c r="D36" s="8" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="E36" s="8" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="F36" s="8" t="s">
         <v>126</v>
       </c>
       <c r="G36" s="22" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="H36" s="22" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="I36" s="8" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="J36" s="11" t="s">
         <v>109</v>
@@ -3638,31 +3638,31 @@
     </row>
     <row r="37" spans="1:26" ht="15.75" customHeight="1">
       <c r="A37" s="32" t="s">
+        <v>300</v>
+      </c>
+      <c r="B37" s="33" t="s">
+        <v>301</v>
+      </c>
+      <c r="C37" s="16" t="s">
         <v>302</v>
       </c>
-      <c r="B37" s="33" t="s">
-        <v>303</v>
-      </c>
-      <c r="C37" s="16" t="s">
-        <v>304</v>
-      </c>
       <c r="D37" s="16" t="s">
-        <v>331</v>
+        <v>328</v>
       </c>
       <c r="E37" s="16" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="F37" s="16" t="s">
         <v>126</v>
       </c>
       <c r="G37" s="32" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="H37" s="32" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="I37" s="16" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="J37" s="34" t="s">
         <v>109</v>
@@ -3686,16 +3686,16 @@
     </row>
     <row r="38" spans="1:26" ht="15.75" customHeight="1">
       <c r="A38" s="5" t="s">
+        <v>305</v>
+      </c>
+      <c r="B38" s="7" t="s">
+        <v>306</v>
+      </c>
+      <c r="C38" s="8" t="s">
         <v>307</v>
       </c>
-      <c r="B38" s="7" t="s">
-        <v>308</v>
-      </c>
-      <c r="C38" s="8" t="s">
-        <v>309</v>
-      </c>
       <c r="D38" s="8" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="E38" s="8" t="s">
         <v>134</v>
@@ -3704,16 +3704,16 @@
         <v>151</v>
       </c>
       <c r="G38" s="5" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="H38" s="5" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="I38" s="8" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="J38" s="11" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="K38" s="12"/>
       <c r="L38" s="12"/>
@@ -3734,32 +3734,32 @@
     </row>
     <row r="39" spans="1:26" ht="15.75" customHeight="1">
       <c r="A39" s="5" t="s">
+        <v>310</v>
+      </c>
+      <c r="B39" s="7" t="s">
+        <v>311</v>
+      </c>
+      <c r="C39" s="8" t="s">
         <v>312</v>
       </c>
-      <c r="B39" s="7" t="s">
-        <v>313</v>
-      </c>
-      <c r="C39" s="8" t="s">
-        <v>314</v>
-      </c>
       <c r="D39" s="8" t="s">
-        <v>332</v>
+        <v>329</v>
       </c>
       <c r="E39" s="8" t="s">
         <v>134</v>
       </c>
       <c r="F39" s="8" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="G39" s="5" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="H39" s="18"/>
       <c r="I39" s="8" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="J39" s="11" t="s">
-        <v>330</v>
+        <v>327</v>
       </c>
     </row>
     <row r="40" spans="1:26" ht="15.75" customHeight="1">

</xml_diff>

<commit_message>
Teach Resources Excel File
</commit_message>
<xml_diff>
--- a/resources/excel/resources-teach.xlsx
+++ b/resources/excel/resources-teach.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="25600" yWindow="0" windowWidth="25600" windowHeight="26740" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="51200" windowHeight="27060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="20190114-Teach-Database" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="445" uniqueCount="335">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="452" uniqueCount="342">
   <si>
     <t>Teach</t>
   </si>
@@ -121,9 +121,6 @@
     <t>Graphic material</t>
   </si>
   <si>
-    <t>https://makelearn.files.wordpress.com/2017/05/screen-shot-2017-05-27-at-4-50-16-pm.png?w=684&amp;h=600&amp;crop=1</t>
-  </si>
-  <si>
     <t>Presentation</t>
   </si>
   <si>
@@ -202,9 +199,6 @@
     <t>Special Education Needs</t>
   </si>
   <si>
-    <t>http://www.scratchjr.org/images/scratchjrlogo.png</t>
-  </si>
-  <si>
     <t xml:space="preserve"> Add "Music"</t>
   </si>
   <si>
@@ -247,9 +241,6 @@
     <t>All targeted languages</t>
   </si>
   <si>
-    <t>https://www.robomindacademy.com/site/images/toplogo.png</t>
-  </si>
-  <si>
     <t>Programming Language</t>
   </si>
   <si>
@@ -292,9 +283,6 @@
     <t>Python</t>
   </si>
   <si>
-    <t>https://codillion.org/wp-content/uploads/2016/09/CodeWeek-FINAL-logo.jpg</t>
-  </si>
-  <si>
     <t>Raspberry Pi</t>
   </si>
   <si>
@@ -325,9 +313,6 @@
     <t>http://codeweek.it/cody-roby-en/ecw-edition/</t>
   </si>
   <si>
-    <t>Codyroby Thumbnail.png</t>
-  </si>
-  <si>
     <t>Computer science; Programming; Coding; Other</t>
   </si>
   <si>
@@ -349,9 +334,6 @@
     <t>https://studio.code.org/courses?view=teacher</t>
   </si>
   <si>
-    <t>https://code.org/images/logo.png</t>
-  </si>
-  <si>
     <t xml:space="preserve">Pre-primary education; Primary school (5-12); Lower secondary school (12-16); Upper secondary school (16-18); </t>
   </si>
   <si>
@@ -373,9 +355,6 @@
     <t xml:space="preserve">http://www.toxicode.fr/learn </t>
   </si>
   <si>
-    <t>Toxicode thumbnail.JPG</t>
-  </si>
-  <si>
     <t>Primary school (5-12); Lower secondary school (12-16);Upper secondary school (16-18)</t>
   </si>
   <si>
@@ -391,9 +370,6 @@
     <t>https://codecombat.com/</t>
   </si>
   <si>
-    <t>https://codecombat.dexecure.net/images/pages/base/logo.png</t>
-  </si>
-  <si>
     <t>Code Avengers</t>
   </si>
   <si>
@@ -409,9 +385,6 @@
     <t>https://www.codeavengers.com/</t>
   </si>
   <si>
-    <t>https://www.codeavengers.com/image/codeavengers_thumb.jpg</t>
-  </si>
-  <si>
     <t xml:space="preserve"> Primary school (5-12); Lower secondary school (12-16); Upper secondary school (16-18); </t>
   </si>
   <si>
@@ -445,9 +418,6 @@
     <t>https://www.freecodecamp.org/</t>
   </si>
   <si>
-    <t>https://secure.meetupstatic.com/photos/event/4/c/b/b/600_468259643.jpeg</t>
-  </si>
-  <si>
     <t xml:space="preserve"> Computer science; Programming; Coding; </t>
   </si>
   <si>
@@ -466,9 +436,6 @@
     <t>https://hackpledge.org/</t>
   </si>
   <si>
-    <t>https://res-2.cloudinary.com/crunchbase-production/image/upload/c_lpad,h_256,w_256,f_auto,q_auto:eco/v1419230398/xckajtsigkzycsd9mbeo.png</t>
-  </si>
-  <si>
     <t xml:space="preserve"> Upper secondary school (16-18); Higher education; Other;</t>
   </si>
   <si>
@@ -484,9 +451,6 @@
     <t>https://csfirst.withgoogle.com/c/cs-first/en/curriculum.html</t>
   </si>
   <si>
-    <t>https://www.chrl.org/wp-content/uploads/2017/08/google-cs-first.png</t>
-  </si>
-  <si>
     <t>Computer science; Programming; Coding; Art; Physical Education; Music; Other</t>
   </si>
   <si>
@@ -523,9 +487,6 @@
     <t>https://education.minecraft.net/</t>
   </si>
   <si>
-    <t>https://i.ytimg.com/vi/Cv6f-2Wlsxg/maxresdefault.jpg</t>
-  </si>
-  <si>
     <t xml:space="preserve">Primary school (5-12); Lower secondary school (12-16); </t>
   </si>
   <si>
@@ -541,9 +502,6 @@
     <t>http://www.glowscript.org/#/user/GlowScriptDemos/folder/Examples/</t>
   </si>
   <si>
-    <t>http://www.glowscript.org/docs/GlowScriptDocs/images/cover.jpg</t>
-  </si>
-  <si>
     <t>Chemistry; Other</t>
   </si>
   <si>
@@ -562,9 +520,6 @@
     <t>https://trinket.io/</t>
   </si>
   <si>
-    <t>https://pbs.twimg.com/profile_images/425621032053923841/0zOVqszZ_400x400.png</t>
-  </si>
-  <si>
     <t xml:space="preserve"> Lower secondary school (12-16); Upper secondary school (16-18);</t>
   </si>
   <si>
@@ -589,9 +544,6 @@
     <t>www.skolskiportal.edu.me</t>
   </si>
   <si>
-    <t>http://www.skolskiportal.edu.me/PublishingImages/skolski-portal3.png</t>
-  </si>
-  <si>
     <t>Kodu GameLab Community</t>
   </si>
   <si>
@@ -607,9 +559,6 @@
     <t>https://www.kodugamelab.com/</t>
   </si>
   <si>
-    <t>https://www.kodugamelab.com/images/top_950.png</t>
-  </si>
-  <si>
     <t>Computer science; Mathematics; Natural sciences; Programming; Coding; Physics; Geology; Other;</t>
   </si>
   <si>
@@ -647,9 +596,6 @@
   </si>
   <si>
     <t>https://onderwijs.vlaanderen.be/nl/zo-denkt-een-computer-programmeren-en-computationeel-denken-in-het-onderwijs</t>
-  </si>
-  <si>
-    <t>https://onderwijs.vlaanderen.be/sites/default/files/paddle_core_plugin_data/branding/logomettekst_versie2_0.png</t>
   </si>
   <si>
     <t xml:space="preserve"> Computer science; Programming; Coding;Other;</t>
@@ -706,9 +652,6 @@
     <t>https://www.programmailfuturo.it/</t>
   </si>
   <si>
-    <t>https://www.programmailfuturo.it/images/logo_pif.png</t>
-  </si>
-  <si>
     <t>Scuola Digitale</t>
   </si>
   <si>
@@ -719,9 +662,6 @@
   </si>
   <si>
     <t>http://www.formazionepnsd.it/competenze-e-contenuti/le-competenze-degli-studenti/</t>
-  </si>
-  <si>
-    <t>http://www.formazionepnsd.it/wp-content/themes/pnsd/img/logo.png</t>
   </si>
   <si>
     <t>Pre-primary education; Primary school (5-12); Lower secondary school (12-16); Other;</t>
@@ -787,9 +727,6 @@
     <t>http://d-clicsnumeriques.org/</t>
   </si>
   <si>
-    <t>https://d-clicsnumeriques.org/wp-content/themes/declic/images/logo.png</t>
-  </si>
-  <si>
     <t xml:space="preserve">Coding; Programming; </t>
   </si>
   <si>
@@ -805,9 +742,6 @@
     <t>https://pixees.fr/classcode-v2/</t>
   </si>
   <si>
-    <t>https://www.inria.fr/var/inria/storage/images/medias/actualites/generales/images-chapo/class-code-logo/1474032-4-fre-FR/class-code-logo_vignette.jpg</t>
-  </si>
-  <si>
     <t xml:space="preserve">Computer science; Coding; Programming; </t>
   </si>
   <si>
@@ -850,9 +784,6 @@
     <t>https://www.agendadulibre.org/</t>
   </si>
   <si>
-    <t>https://www.agendadulibre.org/assets/baby_gnu_adl-463a81820aa2d4ffd8e7210dbce1a19ffcac67ef362aa7b092280c6f95c903fc.png</t>
-  </si>
-  <si>
     <t xml:space="preserve">Computer science; Programming; Coding; </t>
   </si>
   <si>
@@ -868,9 +799,6 @@
     <t>http://www.progetiiger.ee/?q=</t>
   </si>
   <si>
-    <t>http://www.progetiiger.ee/img/pt-logo-kolmnurkne-taust.png</t>
-  </si>
-  <si>
     <t>All you need is code</t>
   </si>
   <si>
@@ -883,9 +811,6 @@
     <t>http://www.allyouneediscode.eu/en/lesson-plans</t>
   </si>
   <si>
-    <t>http://www.cloonlyonns.ie/uploads/3/8/6/4/3864801/8584981.png?600</t>
-  </si>
-  <si>
     <t>Primary school (5-12); Lower secondary school (12-16); Upper secondary school (16-18);</t>
   </si>
   <si>
@@ -904,9 +829,6 @@
     <t>https://csunplugged.org/en/</t>
   </si>
   <si>
-    <t>https://i2.wp.com/www.williamsburgfamilies.com/wp-content/uploads/2018/02/ComputerScienceUnplugged-e1517933665873.jpg?fit=550%2C216&amp;ssl=1</t>
-  </si>
-  <si>
     <t>CCEA Phython</t>
   </si>
   <si>
@@ -922,9 +844,6 @@
     <t>http://ccea.org.uk/training/python</t>
   </si>
   <si>
-    <t>http://ccea.org.uk/sites/all/themes/ccea_subtheme/logo.png</t>
-  </si>
-  <si>
     <t>Computer science; Programming; Coding</t>
   </si>
   <si>
@@ -940,9 +859,6 @@
     <t>https://education.github.com/teachers</t>
   </si>
   <si>
-    <t>https://dwa5x7aod66zk.cloudfront.net/assets/next/wordmark-b2322266c45ea75318d0ea4481ab3c0aaa587af433ead331ba0ec402ad79fde9.svg</t>
-  </si>
-  <si>
     <t>Upper secondary school (16-18); Higher education; Other;</t>
   </si>
   <si>
@@ -956,9 +872,6 @@
   </si>
   <si>
     <t>https://www.bebras.org/?q=about</t>
-  </si>
-  <si>
-    <t>https://www.bebras.org/sites/all/themes/bebrasorgtheme/img/bebras_logo.png</t>
   </si>
   <si>
     <t>European Schoolnet Academy</t>
@@ -1003,9 +916,6 @@
     <t>http://www.europeanschoolnetacademy.eu/web/introducing-computing-in-your-classroom</t>
   </si>
   <si>
-    <t>http://www.europeanschoolnetacademy.eu/image/company_logo?img_id=10939&amp;t=1536081160423</t>
-  </si>
-  <si>
     <t>Kids Kodr</t>
   </si>
   <si>
@@ -1018,9 +928,6 @@
     <t>https://www.kidscodr.com/</t>
   </si>
   <si>
-    <t>https://www.kidscodr.com/assets/logo-09e5a511479dece222ccaf1ae6e3df4b809b51fa5c33fbfb7a54073524c2aa02.png</t>
-  </si>
-  <si>
     <t>Code INTEF</t>
   </si>
   <si>
@@ -1094,13 +1001,127 @@
   </si>
   <si>
     <t>Art; Biology; Chemistry; Computer science; Culture; Economics; Foreign Languages; Geography; Geology; History; Language and Literature; Mathematics; Natural sciences; Physical Education; Physics; Programming; Coding; Other; Other</t>
+  </si>
+  <si>
+    <t>https://s3-eu-west-1.amazonaws.com/codeweek-resources/cMttQZFjF7LwoYKnKQCepuWeGEOmwajlDfCNqGl2.png</t>
+  </si>
+  <si>
+    <t>https://s3-eu-west-1.amazonaws.com/codeweek-resources/3TVDdt1CHD0hH2WWD8SWLOwOtK5B95iffsrkFES4.png</t>
+  </si>
+  <si>
+    <t>https://s3-eu-west-1.amazonaws.com/codeweek-resources/XT3uqwuny8J88OlP1u8PWkeZ3tO3xnabV1vAPhZS.png</t>
+  </si>
+  <si>
+    <t>https://s3-eu-west-1.amazonaws.com/codeweek-resources/W6sk4QE5EzAADXhBM4lWl5XygMHaRXzyo52RhGwO.png</t>
+  </si>
+  <si>
+    <t>https://s3-eu-west-1.amazonaws.com/codeweek-resources/QALx68QLKtCopH02evyUUHtv2pv1U0QHlurXSvx4.png</t>
+  </si>
+  <si>
+    <t>https://s3-eu-west-1.amazonaws.com/codeweek-resources/4pcWUOqqYNaqgWulEroXh5xCpoXbbA83lU107o2a.png</t>
+  </si>
+  <si>
+    <t>https://s3-eu-west-1.amazonaws.com/codeweek-resources/0UArJk7F5gANaQ4JuLuXU57J9d5qSPc8NuZ5X6Wo.png</t>
+  </si>
+  <si>
+    <t>https://s3-eu-west-1.amazonaws.com/codeweek-resources/FnvkFxDvCI0rYlIcQApDMiv1g2J1BEX0iJD5Lc11.png</t>
+  </si>
+  <si>
+    <t>https://s3-eu-west-1.amazonaws.com/codeweek-resources/SKfDQnzt8KFIK2oIL9EfPhmW3mlYQFsfoR6ZJwL3.png</t>
+  </si>
+  <si>
+    <t>https://s3-eu-west-1.amazonaws.com/codeweek-resources/xMtlyOhW02W0FfIygjPRQQ6FPpP4dPwOvgsDx53g.png</t>
+  </si>
+  <si>
+    <t>https://s3-eu-west-1.amazonaws.com/codeweek-resources/6LlsFKLOSs2UJKMMNmxuxskl5nl4j34m0tMqLIJR.png</t>
+  </si>
+  <si>
+    <t>https://s3-eu-west-1.amazonaws.com/codeweek-resources/Q1kKW7JIqChgKbQWakMdiiKQGg0ER8BEwEVy5pis.png</t>
+  </si>
+  <si>
+    <t>https://s3-eu-west-1.amazonaws.com/codeweek-resources/1AStxXDSIVIRrcjMt5wdKwXZED54nqSUOzfNYw07.png</t>
+  </si>
+  <si>
+    <t>https://s3-eu-west-1.amazonaws.com/codeweek-resources/7tsWeA07Y3f7GDK7Yvo8Y8mVCE4kSQHUdFkOKiKK.png</t>
+  </si>
+  <si>
+    <t>https://s3-eu-west-1.amazonaws.com/codeweek-resources/32jpmyOEmzoIBvPw2jdlKdY040IJkyVxoCVpqAOK.png</t>
+  </si>
+  <si>
+    <t>https://s3-eu-west-1.amazonaws.com/codeweek-resources/SIif9kEfqzjRQhz4hdrYaUuCnkQIjHzKFR9DwOjh.jpeg</t>
+  </si>
+  <si>
+    <t>https://s3-eu-west-1.amazonaws.com/codeweek-resources/zuXdism1X78s6mm99B0gRSZHvFigMhZXSRHjkvPY.png</t>
+  </si>
+  <si>
+    <t>https://s3-eu-west-1.amazonaws.com/codeweek-resources/tFwkOZGCaf8wQ6udX2THe9YiHpT8DGYCC34bpwzQ.png</t>
+  </si>
+  <si>
+    <t>https://s3-eu-west-1.amazonaws.com/codeweek-resources/ovtGIvIar93JyqmhHl8JDfjkGBSy0SmhlX5EakR4.png</t>
+  </si>
+  <si>
+    <t>https://s3-eu-west-1.amazonaws.com/codeweek-resources/1BNHbJWjdEC7T3urglufaV3Fqyqda5AyrK3FG24T.png</t>
+  </si>
+  <si>
+    <t>https://s3-eu-west-1.amazonaws.com/codeweek-resources/vwKwE01BF1zApieJkbUHRVtbSftLQshC9yHGaEPK.png</t>
+  </si>
+  <si>
+    <t>https://s3-eu-west-1.amazonaws.com/codeweek-resources/2RzMlRRBYC0aNFChXqCVkQZ6Q9OQ0kJhT40grTvx.png</t>
+  </si>
+  <si>
+    <t>https://s3-eu-west-1.amazonaws.com/codeweek-resources/kmWVffuVUKqxqBA1jXSfWEICThf6HaRk44Z11Yl6.png</t>
+  </si>
+  <si>
+    <t>https://s3-eu-west-1.amazonaws.com/codeweek-resources/gvql6Z9bCFqEKQeAk2iMvsqCdJfsPlDo76x9Kmpa.png</t>
+  </si>
+  <si>
+    <t>https://s3-eu-west-1.amazonaws.com/codeweek-resources/hq1GVepEwiybWprMKzei7RyeCfrdSQI87hOHuqhf.png</t>
+  </si>
+  <si>
+    <t>https://s3-eu-west-1.amazonaws.com/codeweek-resources/0OZ3GQIM4AxepeWS52lDutQKG8TKMYadiaKqvikx.png</t>
+  </si>
+  <si>
+    <t>https://s3-eu-west-1.amazonaws.com/codeweek-resources/kdn5kVibGIBYKYnGZ2T2m7xQSUCMt8nVYd9QD0Vg.png</t>
+  </si>
+  <si>
+    <t>https://s3-eu-west-1.amazonaws.com/codeweek-resources/fRw2EoAJMoYl08Gyo6kSNgZzk9izXwlIfsoTyp9B.png</t>
+  </si>
+  <si>
+    <t>https://s3-eu-west-1.amazonaws.com/codeweek-resources/HQamcU1i8rjSHUApjgFdDizgY0nqpOkQLycWluff.png</t>
+  </si>
+  <si>
+    <t>MV5pmUxwXCe1qTRnsS7ofEajHVZ2FyUBGLVV0eFP.png</t>
+  </si>
+  <si>
+    <t>https://s3-eu-west-1.amazonaws.com/codeweek-resources/7hM2diMQ7cJVPDMRc83GIMslZSKAVC1NV82QTPEd.png</t>
+  </si>
+  <si>
+    <t>https://s3-eu-west-1.amazonaws.com/codeweek-resources/cMKgfWMoU34cY41XxiGv6bhrJ9Nnan5oI6ul0tLg.png</t>
+  </si>
+  <si>
+    <t>https://s3-eu-west-1.amazonaws.com/codeweek-resources/zcvrRGmCLcur0t39uQ6rb2Tv23PW7C1TvC4miD0E.png</t>
+  </si>
+  <si>
+    <t>https://s3-eu-west-1.amazonaws.com/codeweek-resources/OsBW9UfPSjWb5kGASpiYUcYqvkp3jDh4ip92HNR6.png</t>
+  </si>
+  <si>
+    <t>https://s3-eu-west-1.amazonaws.com/codeweek-resources/fwMGz9wYqLjvuTmJfUlqe2fGhJP1gN67V85rihnB.png</t>
+  </si>
+  <si>
+    <t>https://s3-eu-west-1.amazonaws.com/codeweek-resources/86AgvrcBwztSwTD00fGZmKrHxBzS8tyc8mERjbcT.png</t>
+  </si>
+  <si>
+    <t>https://s3-eu-west-1.amazonaws.com/codeweek-resources/57n2HWsBjQyWTQMauuBpFCI6QPgMTNMC32Bqydrg.png</t>
+  </si>
+  <si>
+    <t>https://s3-eu-west-1.amazonaws.com/codeweek-resources/HqxUO9BKi9amiZxmIhtUDMM3NYs0CTVvjPfpqInq.png</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="17" x14ac:knownFonts="1">
+  <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -1194,6 +1215,12 @@
       <u/>
       <sz val="11"/>
       <color theme="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
     </font>
   </fonts>
@@ -1468,14 +1495,24 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="5">
+  <cellStyleXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="48">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1551,6 +1588,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="2" xfId="5" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1571,11 +1609,21 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="5">
+  <cellStyles count="15">
+    <cellStyle name="Lien hypertexte" xfId="5" builtinId="8"/>
     <cellStyle name="Lien hypertexte visité" xfId="1" builtinId="9" hidden="1"/>
     <cellStyle name="Lien hypertexte visité" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Lien hypertexte visité" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Lien hypertexte visité" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="7" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="9" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="11" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="13" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="14" builtinId="9" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1907,8 +1955,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G2" workbookViewId="0">
-      <selection activeCell="I23" sqref="I23"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="H39" sqref="H39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0"/>
@@ -1919,8 +1967,8 @@
     <col min="4" max="4" width="39.1640625" customWidth="1"/>
     <col min="5" max="5" width="20.5" customWidth="1"/>
     <col min="6" max="6" width="34.6640625" customWidth="1"/>
-    <col min="7" max="7" width="34.5" customWidth="1"/>
-    <col min="8" max="8" width="64.33203125" customWidth="1"/>
+    <col min="7" max="7" width="58.33203125" customWidth="1"/>
+    <col min="8" max="8" width="102.6640625" customWidth="1"/>
     <col min="9" max="9" width="61.6640625" customWidth="1"/>
     <col min="10" max="10" width="54" customWidth="1"/>
     <col min="11" max="26" width="8.6640625" customWidth="1"/>
@@ -1976,7 +2024,7 @@
     </row>
     <row r="2" spans="1:26" ht="14">
       <c r="A2" s="5" t="s">
-        <v>330</v>
+        <v>299</v>
       </c>
       <c r="B2" s="7" t="s">
         <v>17</v>
@@ -1997,13 +2045,13 @@
         <v>26</v>
       </c>
       <c r="H2" s="5" t="s">
-        <v>32</v>
+        <v>304</v>
       </c>
       <c r="I2" s="36" t="s">
-        <v>334</v>
+        <v>303</v>
       </c>
       <c r="J2" s="11" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="K2" s="12"/>
       <c r="L2" s="12"/>
@@ -2024,31 +2072,31 @@
     </row>
     <row r="3" spans="1:26" ht="14">
       <c r="A3" s="5" t="s">
-        <v>331</v>
+        <v>300</v>
       </c>
       <c r="B3" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="C3" s="8" t="s">
         <v>43</v>
-      </c>
-      <c r="C3" s="8" t="s">
-        <v>44</v>
       </c>
       <c r="D3" s="8" t="s">
         <v>22</v>
       </c>
       <c r="E3" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="F3" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="F3" s="8" t="s">
-        <v>47</v>
-      </c>
       <c r="G3" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="H3" s="5" t="s">
-        <v>59</v>
+        <v>305</v>
       </c>
       <c r="I3" s="8" t="s">
-        <v>334</v>
+        <v>303</v>
       </c>
       <c r="J3" s="11" t="s">
         <v>12</v>
@@ -2072,34 +2120,34 @@
     </row>
     <row r="4" spans="1:26" ht="28">
       <c r="A4" s="5" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B4" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="D4" s="8" t="s">
         <v>69</v>
-      </c>
-      <c r="C4" s="8" t="s">
-        <v>70</v>
-      </c>
-      <c r="D4" s="8" t="s">
-        <v>71</v>
       </c>
       <c r="E4" s="8" t="s">
         <v>16</v>
       </c>
       <c r="F4" s="8" t="s">
-        <v>316</v>
+        <v>285</v>
       </c>
       <c r="G4" s="5" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="H4" s="5" t="s">
+        <v>306</v>
+      </c>
+      <c r="I4" s="8" t="s">
         <v>74</v>
       </c>
-      <c r="I4" s="8" t="s">
-        <v>77</v>
-      </c>
       <c r="J4" s="11" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="K4" s="12"/>
       <c r="L4" s="12"/>
@@ -2120,34 +2168,34 @@
     </row>
     <row r="5" spans="1:26" ht="28">
       <c r="A5" s="5" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="C5" s="8" t="s">
         <v>21</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="E5" s="8" t="s">
         <v>16</v>
       </c>
       <c r="F5" s="8" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="G5" s="5" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="H5" s="17" t="s">
-        <v>89</v>
+        <v>307</v>
       </c>
       <c r="I5" s="8" t="s">
-        <v>334</v>
+        <v>303</v>
       </c>
       <c r="J5" s="11" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="K5" s="12"/>
       <c r="L5" s="12"/>
@@ -2168,34 +2216,34 @@
     </row>
     <row r="6" spans="1:26" ht="28">
       <c r="A6" s="5" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>318</v>
+        <v>287</v>
       </c>
       <c r="E6" s="8" t="s">
         <v>16</v>
       </c>
       <c r="F6" s="8" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="G6" s="5" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="H6" s="18" t="s">
-        <v>100</v>
+        <v>308</v>
       </c>
       <c r="I6" s="8" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="J6" s="11" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="K6" s="12"/>
       <c r="L6" s="12"/>
@@ -2216,34 +2264,34 @@
     </row>
     <row r="7" spans="1:26" ht="28">
       <c r="A7" s="5" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="D7" s="8" t="s">
         <v>22</v>
       </c>
       <c r="E7" s="8" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="F7" s="8" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="G7" s="5" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="H7" s="5" t="s">
-        <v>108</v>
+        <v>309</v>
       </c>
       <c r="I7" s="8" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="J7" s="11" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="K7" s="12"/>
       <c r="L7" s="12"/>
@@ -2264,34 +2312,34 @@
     </row>
     <row r="8" spans="1:26" ht="28">
       <c r="A8" s="5" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="D8" s="8" t="s">
         <v>22</v>
       </c>
       <c r="E8" s="8" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="F8" s="8" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="G8" s="5" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="H8" s="18" t="s">
-        <v>116</v>
+        <v>310</v>
       </c>
       <c r="I8" s="8" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="J8" s="11" t="s">
-        <v>117</v>
+        <v>110</v>
       </c>
       <c r="K8" s="12"/>
       <c r="L8" s="12"/>
@@ -2312,32 +2360,32 @@
     </row>
     <row r="9" spans="1:26" ht="28">
       <c r="A9" s="5" t="s">
-        <v>118</v>
+        <v>111</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>119</v>
+        <v>112</v>
       </c>
       <c r="C9" s="8" t="s">
-        <v>120</v>
+        <v>113</v>
       </c>
       <c r="D9" s="8" t="s">
         <v>22</v>
       </c>
       <c r="E9" s="8" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="F9" s="8" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="G9" s="5" t="s">
-        <v>121</v>
+        <v>114</v>
       </c>
       <c r="H9" s="5" t="s">
-        <v>122</v>
+        <v>311</v>
       </c>
       <c r="I9" s="8"/>
       <c r="J9" s="11" t="s">
-        <v>319</v>
+        <v>288</v>
       </c>
       <c r="K9" s="12"/>
       <c r="L9" s="12"/>
@@ -2358,32 +2406,32 @@
     </row>
     <row r="10" spans="1:26" ht="28">
       <c r="A10" s="19" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>124</v>
+        <v>116</v>
       </c>
       <c r="C10" s="8" t="s">
-        <v>320</v>
+        <v>289</v>
       </c>
       <c r="D10" s="8" t="s">
         <v>22</v>
       </c>
       <c r="E10" s="8" t="s">
-        <v>125</v>
+        <v>117</v>
       </c>
       <c r="F10" s="8" t="s">
-        <v>126</v>
+        <v>118</v>
       </c>
       <c r="G10" s="5" t="s">
-        <v>127</v>
+        <v>119</v>
       </c>
       <c r="H10" s="5" t="s">
-        <v>128</v>
+        <v>312</v>
       </c>
       <c r="I10" s="8"/>
       <c r="J10" s="20" t="s">
-        <v>129</v>
+        <v>120</v>
       </c>
       <c r="K10" s="12"/>
       <c r="L10" s="12"/>
@@ -2404,32 +2452,34 @@
     </row>
     <row r="11" spans="1:26" ht="28">
       <c r="A11" s="21" t="s">
-        <v>130</v>
+        <v>121</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>131</v>
+        <v>122</v>
       </c>
       <c r="C11" s="8" t="s">
-        <v>132</v>
+        <v>123</v>
       </c>
       <c r="D11" s="8" t="s">
-        <v>133</v>
+        <v>124</v>
       </c>
       <c r="E11" s="8" t="s">
-        <v>134</v>
+        <v>125</v>
       </c>
       <c r="F11" s="8" t="s">
+        <v>118</v>
+      </c>
+      <c r="G11" s="5" t="s">
         <v>126</v>
       </c>
-      <c r="G11" s="5" t="s">
-        <v>135</v>
-      </c>
-      <c r="H11" s="18"/>
+      <c r="H11" s="18" t="s">
+        <v>313</v>
+      </c>
       <c r="I11" s="8" t="s">
-        <v>334</v>
+        <v>303</v>
       </c>
       <c r="J11" s="11" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="K11" s="12"/>
       <c r="L11" s="12"/>
@@ -2450,34 +2500,34 @@
     </row>
     <row r="12" spans="1:26" ht="28">
       <c r="A12" s="5" t="s">
-        <v>136</v>
+        <v>127</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>137</v>
+        <v>128</v>
       </c>
       <c r="C12" s="8" t="s">
-        <v>138</v>
+        <v>129</v>
       </c>
       <c r="D12" s="8" t="s">
         <v>22</v>
       </c>
       <c r="E12" s="8" t="s">
-        <v>322</v>
+        <v>291</v>
       </c>
       <c r="F12" s="8" t="s">
-        <v>126</v>
+        <v>118</v>
       </c>
       <c r="G12" s="5" t="s">
-        <v>139</v>
+        <v>130</v>
       </c>
       <c r="H12" s="5" t="s">
-        <v>140</v>
+        <v>314</v>
       </c>
       <c r="I12" s="8" t="s">
-        <v>141</v>
+        <v>131</v>
       </c>
       <c r="J12" s="11" t="s">
-        <v>142</v>
+        <v>132</v>
       </c>
       <c r="K12" s="12"/>
       <c r="L12" s="12"/>
@@ -2498,34 +2548,34 @@
     </row>
     <row r="13" spans="1:26" ht="14">
       <c r="A13" s="5" t="s">
-        <v>143</v>
+        <v>133</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>144</v>
+        <v>134</v>
       </c>
       <c r="C13" s="8" t="s">
-        <v>145</v>
+        <v>135</v>
       </c>
       <c r="D13" s="8" t="s">
         <v>22</v>
       </c>
       <c r="E13" s="8" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="F13" s="8" t="s">
-        <v>126</v>
+        <v>118</v>
       </c>
       <c r="G13" s="5" t="s">
-        <v>146</v>
+        <v>136</v>
       </c>
       <c r="H13" s="5" t="s">
-        <v>147</v>
+        <v>315</v>
       </c>
       <c r="I13" s="8" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="J13" s="11" t="s">
-        <v>148</v>
+        <v>137</v>
       </c>
       <c r="K13" s="12"/>
       <c r="L13" s="12"/>
@@ -2546,13 +2596,13 @@
     </row>
     <row r="14" spans="1:26" ht="14">
       <c r="A14" s="5" t="s">
-        <v>149</v>
+        <v>138</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>150</v>
+        <v>139</v>
       </c>
       <c r="C14" s="8" t="s">
-        <v>323</v>
+        <v>292</v>
       </c>
       <c r="D14" s="8" t="s">
         <v>22</v>
@@ -2561,19 +2611,19 @@
         <v>16</v>
       </c>
       <c r="F14" s="8" t="s">
-        <v>151</v>
+        <v>140</v>
       </c>
       <c r="G14" s="5" t="s">
-        <v>152</v>
+        <v>141</v>
       </c>
       <c r="H14" s="5" t="s">
-        <v>153</v>
+        <v>316</v>
       </c>
       <c r="I14" s="8" t="s">
-        <v>154</v>
+        <v>142</v>
       </c>
       <c r="J14" s="11" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="K14" s="12"/>
       <c r="L14" s="12"/>
@@ -2594,32 +2644,34 @@
     </row>
     <row r="15" spans="1:26" ht="14">
       <c r="A15" s="22" t="s">
-        <v>155</v>
+        <v>143</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>156</v>
+        <v>144</v>
       </c>
       <c r="C15" s="8" t="s">
-        <v>157</v>
+        <v>145</v>
       </c>
       <c r="D15" s="8" t="s">
         <v>22</v>
       </c>
       <c r="E15" s="8" t="s">
-        <v>158</v>
+        <v>146</v>
       </c>
       <c r="F15" s="8" t="s">
-        <v>126</v>
+        <v>118</v>
       </c>
       <c r="G15" s="5" t="s">
-        <v>159</v>
-      </c>
-      <c r="H15" s="18"/>
+        <v>147</v>
+      </c>
+      <c r="H15" s="18" t="s">
+        <v>317</v>
+      </c>
       <c r="I15" s="8" t="s">
-        <v>160</v>
+        <v>148</v>
       </c>
       <c r="J15" s="11" t="s">
-        <v>161</v>
+        <v>149</v>
       </c>
       <c r="K15" s="12"/>
       <c r="L15" s="12"/>
@@ -2640,34 +2692,34 @@
     </row>
     <row r="16" spans="1:26" ht="14">
       <c r="A16" s="5" t="s">
-        <v>162</v>
+        <v>150</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>163</v>
+        <v>151</v>
       </c>
       <c r="C16" s="8" t="s">
-        <v>324</v>
+        <v>293</v>
       </c>
       <c r="D16" s="8" t="s">
         <v>22</v>
       </c>
       <c r="E16" s="8" t="s">
-        <v>164</v>
+        <v>152</v>
       </c>
       <c r="F16" s="8" t="s">
-        <v>126</v>
+        <v>118</v>
       </c>
       <c r="G16" s="5" t="s">
-        <v>165</v>
-      </c>
-      <c r="H16" s="5" t="s">
-        <v>166</v>
+        <v>153</v>
+      </c>
+      <c r="H16" s="37" t="s">
+        <v>319</v>
       </c>
       <c r="I16" s="8" t="s">
-        <v>333</v>
+        <v>302</v>
       </c>
       <c r="J16" s="11" t="s">
-        <v>167</v>
+        <v>154</v>
       </c>
       <c r="K16" s="12"/>
       <c r="L16" s="12"/>
@@ -2688,34 +2740,34 @@
     </row>
     <row r="17" spans="1:26" ht="14">
       <c r="A17" s="5" t="s">
-        <v>168</v>
+        <v>155</v>
       </c>
       <c r="B17" s="7" t="s">
-        <v>169</v>
+        <v>156</v>
       </c>
       <c r="C17" s="8" t="s">
-        <v>157</v>
+        <v>145</v>
       </c>
       <c r="D17" s="8" t="s">
         <v>22</v>
       </c>
       <c r="E17" s="8" t="s">
-        <v>170</v>
+        <v>157</v>
       </c>
       <c r="F17" s="8" t="s">
-        <v>126</v>
+        <v>118</v>
       </c>
       <c r="G17" s="5" t="s">
-        <v>171</v>
+        <v>158</v>
       </c>
       <c r="H17" s="5" t="s">
-        <v>172</v>
+        <v>318</v>
       </c>
       <c r="I17" s="8" t="s">
-        <v>173</v>
+        <v>159</v>
       </c>
       <c r="J17" s="11" t="s">
-        <v>174</v>
+        <v>160</v>
       </c>
       <c r="K17" s="12"/>
       <c r="L17" s="12"/>
@@ -2736,32 +2788,32 @@
     </row>
     <row r="18" spans="1:26" ht="14">
       <c r="A18" s="5" t="s">
-        <v>175</v>
+        <v>161</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>176</v>
+        <v>162</v>
       </c>
       <c r="C18" s="8" t="s">
-        <v>157</v>
+        <v>145</v>
       </c>
       <c r="D18" s="8" t="s">
         <v>22</v>
       </c>
       <c r="E18" s="8" t="s">
-        <v>177</v>
+        <v>163</v>
       </c>
       <c r="F18" s="8" t="s">
-        <v>126</v>
+        <v>118</v>
       </c>
       <c r="G18" s="5" t="s">
-        <v>178</v>
+        <v>164</v>
       </c>
       <c r="H18" s="5" t="s">
-        <v>179</v>
+        <v>320</v>
       </c>
       <c r="I18" s="8"/>
       <c r="J18" s="11" t="s">
-        <v>180</v>
+        <v>165</v>
       </c>
       <c r="K18" s="12"/>
       <c r="L18" s="12"/>
@@ -2782,34 +2834,34 @@
     </row>
     <row r="19" spans="1:26" ht="42">
       <c r="A19" s="5" t="s">
-        <v>181</v>
+        <v>166</v>
       </c>
       <c r="B19" s="23" t="s">
-        <v>182</v>
+        <v>167</v>
       </c>
       <c r="C19" s="8" t="s">
-        <v>183</v>
+        <v>168</v>
       </c>
       <c r="D19" s="8" t="s">
-        <v>184</v>
+        <v>169</v>
       </c>
       <c r="E19" s="8" t="s">
-        <v>185</v>
+        <v>170</v>
       </c>
       <c r="F19" s="8" t="s">
-        <v>186</v>
+        <v>171</v>
       </c>
       <c r="G19" s="22" t="s">
-        <v>187</v>
+        <v>172</v>
       </c>
       <c r="H19" s="22" t="s">
-        <v>188</v>
+        <v>321</v>
       </c>
       <c r="I19" s="8" t="s">
-        <v>332</v>
+        <v>301</v>
       </c>
       <c r="J19" s="11" t="s">
-        <v>325</v>
+        <v>294</v>
       </c>
       <c r="K19" s="12"/>
       <c r="L19" s="12"/>
@@ -2830,34 +2882,34 @@
     </row>
     <row r="20" spans="1:26" ht="28">
       <c r="A20" s="5" t="s">
-        <v>189</v>
+        <v>173</v>
       </c>
       <c r="B20" s="7" t="s">
-        <v>190</v>
+        <v>174</v>
       </c>
       <c r="C20" s="8" t="s">
-        <v>191</v>
+        <v>175</v>
       </c>
       <c r="D20" s="8" t="s">
-        <v>184</v>
+        <v>169</v>
       </c>
       <c r="E20" s="8" t="s">
         <v>23</v>
       </c>
       <c r="F20" s="8" t="s">
-        <v>192</v>
+        <v>176</v>
       </c>
       <c r="G20" s="5" t="s">
-        <v>193</v>
+        <v>177</v>
       </c>
       <c r="H20" s="5" t="s">
-        <v>194</v>
+        <v>322</v>
       </c>
       <c r="I20" s="8" t="s">
-        <v>195</v>
+        <v>178</v>
       </c>
       <c r="J20" s="11" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="K20" s="12"/>
       <c r="L20" s="12"/>
@@ -2878,32 +2930,34 @@
     </row>
     <row r="21" spans="1:26" ht="15.75" customHeight="1">
       <c r="A21" s="5" t="s">
-        <v>196</v>
+        <v>179</v>
       </c>
       <c r="B21" s="7" t="s">
-        <v>197</v>
+        <v>180</v>
       </c>
       <c r="C21" s="8" t="s">
-        <v>198</v>
+        <v>181</v>
       </c>
       <c r="D21" s="8" t="s">
-        <v>199</v>
+        <v>182</v>
       </c>
       <c r="E21" s="8" t="s">
-        <v>200</v>
+        <v>183</v>
       </c>
       <c r="F21" s="24" t="s">
-        <v>201</v>
+        <v>184</v>
       </c>
       <c r="G21" s="5" t="s">
-        <v>202</v>
-      </c>
-      <c r="H21" s="25"/>
+        <v>185</v>
+      </c>
+      <c r="H21" s="25" t="s">
+        <v>323</v>
+      </c>
       <c r="I21" s="8" t="s">
-        <v>203</v>
+        <v>186</v>
       </c>
       <c r="J21" s="11" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="K21" s="12"/>
       <c r="L21" s="12"/>
@@ -2924,34 +2978,34 @@
     </row>
     <row r="22" spans="1:26" ht="15.75" customHeight="1">
       <c r="A22" s="5" t="s">
-        <v>204</v>
+        <v>187</v>
       </c>
       <c r="B22" s="7" t="s">
-        <v>205</v>
+        <v>188</v>
       </c>
       <c r="C22" s="8" t="s">
-        <v>206</v>
+        <v>189</v>
       </c>
       <c r="D22" s="8" t="s">
-        <v>184</v>
+        <v>169</v>
       </c>
       <c r="E22" s="8" t="s">
-        <v>200</v>
+        <v>183</v>
       </c>
       <c r="F22" s="8" t="s">
-        <v>317</v>
+        <v>286</v>
       </c>
       <c r="G22" s="5" t="s">
-        <v>207</v>
+        <v>190</v>
       </c>
       <c r="H22" s="5" t="s">
-        <v>208</v>
+        <v>324</v>
       </c>
       <c r="I22" s="8" t="s">
-        <v>209</v>
+        <v>191</v>
       </c>
       <c r="J22" s="11" t="s">
-        <v>210</v>
+        <v>192</v>
       </c>
       <c r="K22" s="12"/>
       <c r="L22" s="12"/>
@@ -2972,32 +3026,34 @@
     </row>
     <row r="23" spans="1:26" ht="15.75" customHeight="1">
       <c r="A23" s="5" t="s">
-        <v>211</v>
+        <v>193</v>
       </c>
       <c r="B23" s="23" t="s">
-        <v>212</v>
+        <v>194</v>
       </c>
       <c r="C23" s="8" t="s">
-        <v>213</v>
+        <v>195</v>
       </c>
       <c r="D23" s="7" t="s">
-        <v>184</v>
+        <v>169</v>
       </c>
       <c r="E23" s="8" t="s">
-        <v>214</v>
+        <v>196</v>
       </c>
       <c r="F23" s="8" t="s">
-        <v>215</v>
+        <v>197</v>
       </c>
       <c r="G23" s="22" t="s">
-        <v>216</v>
-      </c>
-      <c r="H23" s="26"/>
+        <v>198</v>
+      </c>
+      <c r="H23" s="26" t="s">
+        <v>325</v>
+      </c>
       <c r="I23" s="8" t="s">
-        <v>217</v>
+        <v>199</v>
       </c>
       <c r="J23" s="20" t="s">
-        <v>218</v>
+        <v>200</v>
       </c>
       <c r="K23" s="12"/>
       <c r="L23" s="12"/>
@@ -3018,34 +3074,34 @@
     </row>
     <row r="24" spans="1:26" ht="15.75" customHeight="1">
       <c r="A24" s="5" t="s">
-        <v>219</v>
+        <v>201</v>
       </c>
       <c r="B24" s="23" t="s">
-        <v>220</v>
+        <v>202</v>
       </c>
       <c r="C24" s="8" t="s">
-        <v>221</v>
+        <v>203</v>
       </c>
       <c r="D24" s="7" t="s">
-        <v>184</v>
+        <v>169</v>
       </c>
       <c r="E24" s="8" t="s">
-        <v>200</v>
+        <v>183</v>
       </c>
       <c r="F24" s="8" t="s">
-        <v>222</v>
+        <v>204</v>
       </c>
       <c r="G24" s="22" t="s">
-        <v>223</v>
+        <v>205</v>
       </c>
       <c r="H24" s="22" t="s">
-        <v>224</v>
+        <v>326</v>
       </c>
       <c r="I24" s="8" t="s">
-        <v>217</v>
+        <v>199</v>
       </c>
       <c r="J24" s="20" t="s">
-        <v>210</v>
+        <v>192</v>
       </c>
       <c r="K24" s="12"/>
       <c r="L24" s="12"/>
@@ -3066,34 +3122,34 @@
     </row>
     <row r="25" spans="1:26" ht="15.75" customHeight="1">
       <c r="A25" s="5" t="s">
-        <v>225</v>
+        <v>206</v>
       </c>
       <c r="B25" s="23" t="s">
-        <v>226</v>
+        <v>207</v>
       </c>
       <c r="C25" s="8" t="s">
-        <v>206</v>
+        <v>189</v>
       </c>
       <c r="D25" s="7" t="s">
-        <v>227</v>
+        <v>208</v>
       </c>
       <c r="E25" s="8" t="s">
-        <v>200</v>
+        <v>183</v>
       </c>
       <c r="F25" s="8" t="s">
-        <v>222</v>
+        <v>204</v>
       </c>
       <c r="G25" s="22" t="s">
-        <v>228</v>
+        <v>209</v>
       </c>
       <c r="H25" s="22" t="s">
-        <v>229</v>
+        <v>327</v>
       </c>
       <c r="I25" s="8" t="s">
-        <v>217</v>
+        <v>199</v>
       </c>
       <c r="J25" s="20" t="s">
-        <v>230</v>
+        <v>210</v>
       </c>
       <c r="K25" s="12"/>
       <c r="L25" s="12"/>
@@ -3114,32 +3170,34 @@
     </row>
     <row r="26" spans="1:26" ht="15.75" customHeight="1">
       <c r="A26" s="17" t="s">
-        <v>231</v>
+        <v>211</v>
       </c>
       <c r="B26" s="23" t="s">
-        <v>232</v>
+        <v>212</v>
       </c>
       <c r="C26" s="8" t="s">
-        <v>233</v>
+        <v>213</v>
       </c>
       <c r="D26" s="8" t="s">
-        <v>184</v>
+        <v>169</v>
       </c>
       <c r="E26" s="8" t="s">
-        <v>200</v>
+        <v>183</v>
       </c>
       <c r="F26" s="8" t="s">
-        <v>234</v>
+        <v>214</v>
       </c>
       <c r="G26" s="22" t="s">
-        <v>235</v>
-      </c>
-      <c r="H26" s="27"/>
+        <v>215</v>
+      </c>
+      <c r="H26" s="27" t="s">
+        <v>328</v>
+      </c>
       <c r="I26" s="8" t="s">
-        <v>217</v>
+        <v>199</v>
       </c>
       <c r="J26" s="20" t="s">
-        <v>236</v>
+        <v>216</v>
       </c>
       <c r="K26" s="12"/>
       <c r="L26" s="12"/>
@@ -3160,34 +3218,34 @@
     </row>
     <row r="27" spans="1:26" ht="15.75" customHeight="1">
       <c r="A27" s="5" t="s">
-        <v>237</v>
+        <v>217</v>
       </c>
       <c r="B27" s="23" t="s">
-        <v>238</v>
+        <v>218</v>
       </c>
       <c r="C27" s="8" t="s">
-        <v>132</v>
+        <v>123</v>
       </c>
       <c r="D27" s="8" t="s">
-        <v>239</v>
+        <v>219</v>
       </c>
       <c r="E27" s="8" t="s">
-        <v>200</v>
+        <v>183</v>
       </c>
       <c r="F27" s="8" t="s">
-        <v>240</v>
+        <v>220</v>
       </c>
       <c r="G27" s="22" t="s">
-        <v>241</v>
+        <v>221</v>
       </c>
       <c r="H27" s="22" t="s">
-        <v>242</v>
+        <v>329</v>
       </c>
       <c r="I27" s="8" t="s">
-        <v>243</v>
+        <v>222</v>
       </c>
       <c r="J27" s="11" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="K27" s="12"/>
       <c r="L27" s="12"/>
@@ -3208,34 +3266,34 @@
     </row>
     <row r="28" spans="1:26" ht="15.75" customHeight="1">
       <c r="A28" s="5" t="s">
-        <v>244</v>
+        <v>223</v>
       </c>
       <c r="B28" s="23" t="s">
-        <v>245</v>
+        <v>224</v>
       </c>
       <c r="C28" s="36" t="s">
-        <v>321</v>
+        <v>290</v>
       </c>
       <c r="D28" s="16" t="s">
-        <v>246</v>
+        <v>225</v>
       </c>
       <c r="E28" s="8" t="s">
-        <v>200</v>
+        <v>183</v>
       </c>
       <c r="F28" s="8" t="s">
-        <v>240</v>
+        <v>220</v>
       </c>
       <c r="G28" s="22" t="s">
-        <v>247</v>
+        <v>226</v>
       </c>
       <c r="H28" s="22" t="s">
-        <v>248</v>
+        <v>330</v>
       </c>
       <c r="I28" s="8" t="s">
-        <v>249</v>
+        <v>227</v>
       </c>
       <c r="J28" s="11" t="s">
-        <v>210</v>
+        <v>192</v>
       </c>
       <c r="K28" s="12"/>
       <c r="L28" s="12"/>
@@ -3256,32 +3314,34 @@
     </row>
     <row r="29" spans="1:26" ht="15.75" customHeight="1">
       <c r="A29" s="5" t="s">
-        <v>250</v>
+        <v>228</v>
       </c>
       <c r="B29" s="23" t="s">
-        <v>251</v>
+        <v>229</v>
       </c>
       <c r="C29" s="28" t="s">
-        <v>252</v>
+        <v>230</v>
       </c>
       <c r="D29" s="8" t="s">
-        <v>253</v>
+        <v>231</v>
       </c>
       <c r="E29" s="29" t="s">
-        <v>254</v>
+        <v>232</v>
       </c>
       <c r="F29" s="8" t="s">
-        <v>255</v>
+        <v>233</v>
       </c>
       <c r="G29" s="22" t="s">
-        <v>256</v>
-      </c>
-      <c r="H29" s="30"/>
+        <v>234</v>
+      </c>
+      <c r="H29" s="30" t="s">
+        <v>331</v>
+      </c>
       <c r="I29" s="8" t="s">
-        <v>257</v>
+        <v>235</v>
       </c>
       <c r="J29" s="11" t="s">
-        <v>327</v>
+        <v>296</v>
       </c>
       <c r="K29" s="12"/>
       <c r="L29" s="12"/>
@@ -3302,34 +3362,34 @@
     </row>
     <row r="30" spans="1:26" ht="15.75" customHeight="1">
       <c r="A30" s="5" t="s">
-        <v>258</v>
+        <v>236</v>
       </c>
       <c r="B30" s="7" t="s">
-        <v>259</v>
+        <v>237</v>
       </c>
       <c r="C30" s="8" t="s">
-        <v>260</v>
+        <v>238</v>
       </c>
       <c r="D30" s="31" t="s">
-        <v>261</v>
+        <v>239</v>
       </c>
       <c r="E30" s="8" t="s">
-        <v>200</v>
+        <v>183</v>
       </c>
       <c r="F30" s="8" t="s">
+        <v>220</v>
+      </c>
+      <c r="G30" s="5" t="s">
         <v>240</v>
       </c>
-      <c r="G30" s="5" t="s">
-        <v>262</v>
-      </c>
       <c r="H30" s="5" t="s">
-        <v>263</v>
+        <v>333</v>
       </c>
       <c r="I30" s="8" t="s">
-        <v>264</v>
+        <v>241</v>
       </c>
       <c r="J30" s="11" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="K30" s="12"/>
       <c r="L30" s="12"/>
@@ -3350,34 +3410,34 @@
     </row>
     <row r="31" spans="1:26" ht="15.75" customHeight="1">
       <c r="A31" s="5" t="s">
-        <v>265</v>
+        <v>242</v>
       </c>
       <c r="B31" s="7" t="s">
-        <v>266</v>
+        <v>243</v>
       </c>
       <c r="C31" s="8" t="s">
-        <v>157</v>
+        <v>145</v>
       </c>
       <c r="D31" s="8" t="s">
-        <v>243</v>
+        <v>222</v>
       </c>
       <c r="E31" s="28" t="s">
-        <v>200</v>
+        <v>183</v>
       </c>
       <c r="F31" s="8" t="s">
-        <v>267</v>
+        <v>244</v>
       </c>
       <c r="G31" s="5" t="s">
-        <v>268</v>
+        <v>245</v>
       </c>
       <c r="H31" s="5" t="s">
-        <v>269</v>
+        <v>332</v>
       </c>
       <c r="I31" s="8" t="s">
-        <v>257</v>
+        <v>235</v>
       </c>
       <c r="J31" s="11" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="K31" s="12"/>
       <c r="L31" s="12"/>
@@ -3398,34 +3458,34 @@
     </row>
     <row r="32" spans="1:26" ht="15.75" customHeight="1">
       <c r="A32" s="5" t="s">
-        <v>270</v>
+        <v>246</v>
       </c>
       <c r="B32" s="7" t="s">
-        <v>271</v>
+        <v>247</v>
       </c>
       <c r="C32" s="8" t="s">
-        <v>272</v>
+        <v>248</v>
       </c>
       <c r="D32" s="8" t="s">
-        <v>261</v>
+        <v>239</v>
       </c>
       <c r="E32" s="8" t="s">
-        <v>200</v>
+        <v>183</v>
       </c>
       <c r="F32" s="8" t="s">
-        <v>126</v>
+        <v>118</v>
       </c>
       <c r="G32" s="5" t="s">
-        <v>273</v>
+        <v>249</v>
       </c>
       <c r="H32" s="5" t="s">
-        <v>274</v>
+        <v>334</v>
       </c>
       <c r="I32" s="8" t="s">
-        <v>257</v>
+        <v>235</v>
       </c>
       <c r="J32" s="11" t="s">
-        <v>275</v>
+        <v>250</v>
       </c>
       <c r="K32" s="12"/>
       <c r="L32" s="12"/>
@@ -3446,34 +3506,34 @@
     </row>
     <row r="33" spans="1:26" ht="15.75" customHeight="1">
       <c r="A33" s="5" t="s">
-        <v>276</v>
+        <v>251</v>
       </c>
       <c r="B33" s="7" t="s">
-        <v>277</v>
+        <v>252</v>
       </c>
       <c r="C33" s="8" t="s">
-        <v>278</v>
+        <v>253</v>
       </c>
       <c r="D33" s="8" t="s">
-        <v>279</v>
+        <v>254</v>
       </c>
       <c r="E33" s="8" t="s">
-        <v>200</v>
+        <v>183</v>
       </c>
       <c r="F33" s="8" t="s">
-        <v>126</v>
+        <v>118</v>
       </c>
       <c r="G33" s="5" t="s">
-        <v>280</v>
+        <v>255</v>
       </c>
       <c r="H33" s="5" t="s">
-        <v>281</v>
+        <v>335</v>
       </c>
       <c r="I33" s="8" t="s">
-        <v>257</v>
+        <v>235</v>
       </c>
       <c r="J33" s="11" t="s">
-        <v>326</v>
+        <v>295</v>
       </c>
       <c r="K33" s="12"/>
       <c r="L33" s="12"/>
@@ -3494,34 +3554,34 @@
     </row>
     <row r="34" spans="1:26" ht="15.75" customHeight="1">
       <c r="A34" s="5" t="s">
-        <v>282</v>
+        <v>256</v>
       </c>
       <c r="B34" s="7" t="s">
-        <v>283</v>
+        <v>257</v>
       </c>
       <c r="C34" s="8" t="s">
-        <v>284</v>
+        <v>258</v>
       </c>
       <c r="D34" s="8" t="s">
-        <v>243</v>
+        <v>222</v>
       </c>
       <c r="E34" s="8" t="s">
-        <v>285</v>
+        <v>259</v>
       </c>
       <c r="F34" s="8" t="s">
-        <v>126</v>
+        <v>118</v>
       </c>
       <c r="G34" s="5" t="s">
-        <v>286</v>
+        <v>260</v>
       </c>
       <c r="H34" s="5" t="s">
-        <v>287</v>
+        <v>336</v>
       </c>
       <c r="I34" s="8" t="s">
-        <v>288</v>
+        <v>261</v>
       </c>
       <c r="J34" s="11" t="s">
-        <v>289</v>
+        <v>262</v>
       </c>
       <c r="K34" s="12"/>
       <c r="L34" s="12"/>
@@ -3542,34 +3602,34 @@
     </row>
     <row r="35" spans="1:26" ht="15.75" customHeight="1">
       <c r="A35" s="5" t="s">
-        <v>290</v>
+        <v>263</v>
       </c>
       <c r="B35" s="7" t="s">
-        <v>291</v>
+        <v>264</v>
       </c>
       <c r="C35" s="8" t="s">
-        <v>157</v>
+        <v>145</v>
       </c>
       <c r="D35" s="8" t="s">
         <v>22</v>
       </c>
       <c r="E35" s="8" t="s">
-        <v>200</v>
+        <v>183</v>
       </c>
       <c r="F35" s="8" t="s">
-        <v>126</v>
+        <v>118</v>
       </c>
       <c r="G35" s="5" t="s">
-        <v>292</v>
+        <v>265</v>
       </c>
       <c r="H35" s="5" t="s">
-        <v>293</v>
+        <v>337</v>
       </c>
       <c r="I35" s="8" t="s">
-        <v>257</v>
+        <v>235</v>
       </c>
       <c r="J35" s="11" t="s">
-        <v>294</v>
+        <v>266</v>
       </c>
       <c r="K35" s="12"/>
       <c r="L35" s="12"/>
@@ -3590,34 +3650,34 @@
     </row>
     <row r="36" spans="1:26" ht="15.75" customHeight="1">
       <c r="A36" s="5" t="s">
-        <v>295</v>
+        <v>267</v>
       </c>
       <c r="B36" s="23" t="s">
-        <v>296</v>
+        <v>268</v>
       </c>
       <c r="C36" s="8" t="s">
-        <v>132</v>
+        <v>123</v>
       </c>
       <c r="D36" s="8" t="s">
-        <v>297</v>
+        <v>269</v>
       </c>
       <c r="E36" s="8" t="s">
-        <v>200</v>
+        <v>183</v>
       </c>
       <c r="F36" s="8" t="s">
-        <v>126</v>
+        <v>118</v>
       </c>
       <c r="G36" s="22" t="s">
-        <v>298</v>
+        <v>270</v>
       </c>
       <c r="H36" s="22" t="s">
-        <v>299</v>
+        <v>338</v>
       </c>
       <c r="I36" s="8" t="s">
-        <v>257</v>
+        <v>235</v>
       </c>
       <c r="J36" s="11" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="K36" s="12"/>
       <c r="L36" s="12"/>
@@ -3638,34 +3698,34 @@
     </row>
     <row r="37" spans="1:26" ht="15.75" customHeight="1">
       <c r="A37" s="32" t="s">
-        <v>300</v>
+        <v>271</v>
       </c>
       <c r="B37" s="33" t="s">
-        <v>301</v>
+        <v>272</v>
       </c>
       <c r="C37" s="16" t="s">
-        <v>302</v>
+        <v>273</v>
       </c>
       <c r="D37" s="16" t="s">
-        <v>328</v>
+        <v>297</v>
       </c>
       <c r="E37" s="16" t="s">
-        <v>200</v>
+        <v>183</v>
       </c>
       <c r="F37" s="16" t="s">
-        <v>126</v>
+        <v>118</v>
       </c>
       <c r="G37" s="32" t="s">
-        <v>303</v>
+        <v>274</v>
       </c>
       <c r="H37" s="32" t="s">
-        <v>304</v>
+        <v>339</v>
       </c>
       <c r="I37" s="16" t="s">
-        <v>257</v>
+        <v>235</v>
       </c>
       <c r="J37" s="34" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="K37" s="12"/>
       <c r="L37" s="12"/>
@@ -3686,34 +3746,34 @@
     </row>
     <row r="38" spans="1:26" ht="15.75" customHeight="1">
       <c r="A38" s="5" t="s">
-        <v>305</v>
+        <v>275</v>
       </c>
       <c r="B38" s="7" t="s">
-        <v>306</v>
+        <v>276</v>
       </c>
       <c r="C38" s="8" t="s">
-        <v>307</v>
+        <v>277</v>
       </c>
       <c r="D38" s="8" t="s">
-        <v>261</v>
+        <v>239</v>
       </c>
       <c r="E38" s="8" t="s">
-        <v>134</v>
+        <v>125</v>
       </c>
       <c r="F38" s="8" t="s">
-        <v>151</v>
+        <v>140</v>
       </c>
       <c r="G38" s="5" t="s">
-        <v>308</v>
+        <v>278</v>
       </c>
       <c r="H38" s="5" t="s">
-        <v>309</v>
+        <v>340</v>
       </c>
       <c r="I38" s="8" t="s">
-        <v>243</v>
+        <v>222</v>
       </c>
       <c r="J38" s="11" t="s">
-        <v>218</v>
+        <v>200</v>
       </c>
       <c r="K38" s="12"/>
       <c r="L38" s="12"/>
@@ -3734,32 +3794,34 @@
     </row>
     <row r="39" spans="1:26" ht="15.75" customHeight="1">
       <c r="A39" s="5" t="s">
-        <v>310</v>
+        <v>279</v>
       </c>
       <c r="B39" s="7" t="s">
-        <v>311</v>
+        <v>280</v>
       </c>
       <c r="C39" s="8" t="s">
-        <v>312</v>
+        <v>281</v>
       </c>
       <c r="D39" s="8" t="s">
-        <v>329</v>
+        <v>298</v>
       </c>
       <c r="E39" s="8" t="s">
-        <v>134</v>
+        <v>125</v>
       </c>
       <c r="F39" s="8" t="s">
-        <v>313</v>
+        <v>282</v>
       </c>
       <c r="G39" s="5" t="s">
-        <v>314</v>
-      </c>
-      <c r="H39" s="18"/>
+        <v>283</v>
+      </c>
+      <c r="H39" s="18" t="s">
+        <v>341</v>
+      </c>
       <c r="I39" s="8" t="s">
-        <v>315</v>
+        <v>284</v>
       </c>
       <c r="J39" s="11" t="s">
-        <v>327</v>
+        <v>296</v>
       </c>
     </row>
     <row r="40" spans="1:26" ht="15.75" customHeight="1">
@@ -15299,109 +15361,82 @@
   <hyperlinks>
     <hyperlink ref="A2" r:id="rId1" display="Scatch by MIT"/>
     <hyperlink ref="G2" r:id="rId2"/>
-    <hyperlink ref="H2" r:id="rId3"/>
-    <hyperlink ref="A3" r:id="rId4" display="Scatch Jr by MIT"/>
-    <hyperlink ref="G3" r:id="rId5"/>
-    <hyperlink ref="H3" r:id="rId6"/>
-    <hyperlink ref="A4" r:id="rId7"/>
-    <hyperlink ref="G4" r:id="rId8"/>
-    <hyperlink ref="H4" r:id="rId9"/>
-    <hyperlink ref="G5" r:id="rId10"/>
-    <hyperlink ref="H5" r:id="rId11"/>
-    <hyperlink ref="A6" r:id="rId12"/>
-    <hyperlink ref="G6" r:id="rId13"/>
-    <hyperlink ref="A7" r:id="rId14"/>
-    <hyperlink ref="G7" r:id="rId15"/>
-    <hyperlink ref="H7" r:id="rId16"/>
-    <hyperlink ref="G8" r:id="rId17"/>
-    <hyperlink ref="A9" r:id="rId18"/>
-    <hyperlink ref="G9" r:id="rId19"/>
-    <hyperlink ref="H9" r:id="rId20"/>
-    <hyperlink ref="A10" r:id="rId21"/>
-    <hyperlink ref="G10" r:id="rId22"/>
-    <hyperlink ref="H10" r:id="rId23"/>
-    <hyperlink ref="A11" r:id="rId24"/>
-    <hyperlink ref="G11" r:id="rId25"/>
-    <hyperlink ref="A12" r:id="rId26"/>
-    <hyperlink ref="G12" r:id="rId27"/>
-    <hyperlink ref="H12" r:id="rId28"/>
-    <hyperlink ref="A13" r:id="rId29"/>
-    <hyperlink ref="G13" r:id="rId30"/>
-    <hyperlink ref="H13" r:id="rId31"/>
-    <hyperlink ref="A14" r:id="rId32"/>
-    <hyperlink ref="G14" r:id="rId33"/>
-    <hyperlink ref="H14" r:id="rId34"/>
-    <hyperlink ref="A15" r:id="rId35" location="/"/>
-    <hyperlink ref="G15" r:id="rId36" location="/"/>
-    <hyperlink ref="A16" r:id="rId37"/>
-    <hyperlink ref="G16" r:id="rId38"/>
-    <hyperlink ref="H16" r:id="rId39"/>
-    <hyperlink ref="A17" r:id="rId40" location="/user/GlowScriptDemos/folder/Examples/"/>
-    <hyperlink ref="G17" r:id="rId41" location="/user/GlowScriptDemos/folder/Examples/"/>
-    <hyperlink ref="H17" r:id="rId42"/>
-    <hyperlink ref="A18" r:id="rId43"/>
-    <hyperlink ref="G18" r:id="rId44"/>
-    <hyperlink ref="H18" r:id="rId45"/>
-    <hyperlink ref="A19" r:id="rId46"/>
-    <hyperlink ref="G19" r:id="rId47"/>
-    <hyperlink ref="H19" r:id="rId48"/>
-    <hyperlink ref="A20" r:id="rId49"/>
-    <hyperlink ref="G20" r:id="rId50"/>
-    <hyperlink ref="H20" r:id="rId51"/>
-    <hyperlink ref="A21" r:id="rId52"/>
-    <hyperlink ref="G21" r:id="rId53"/>
-    <hyperlink ref="A22" r:id="rId54"/>
-    <hyperlink ref="G22" r:id="rId55"/>
-    <hyperlink ref="H22" r:id="rId56"/>
-    <hyperlink ref="A23" r:id="rId57"/>
-    <hyperlink ref="G23" r:id="rId58"/>
-    <hyperlink ref="A24" r:id="rId59"/>
-    <hyperlink ref="G24" r:id="rId60"/>
-    <hyperlink ref="H24" r:id="rId61"/>
-    <hyperlink ref="A25" r:id="rId62"/>
-    <hyperlink ref="G25" r:id="rId63"/>
-    <hyperlink ref="H25" r:id="rId64"/>
-    <hyperlink ref="A26" r:id="rId65"/>
-    <hyperlink ref="G26" r:id="rId66"/>
-    <hyperlink ref="A27" r:id="rId67"/>
-    <hyperlink ref="G27" r:id="rId68"/>
-    <hyperlink ref="H27" r:id="rId69"/>
-    <hyperlink ref="A28" r:id="rId70"/>
-    <hyperlink ref="G28" r:id="rId71"/>
-    <hyperlink ref="H28" r:id="rId72"/>
-    <hyperlink ref="A29" r:id="rId73"/>
-    <hyperlink ref="G29" r:id="rId74"/>
-    <hyperlink ref="A30" r:id="rId75"/>
-    <hyperlink ref="G30" r:id="rId76"/>
-    <hyperlink ref="H30" r:id="rId77"/>
-    <hyperlink ref="A31" r:id="rId78"/>
-    <hyperlink ref="G31" r:id="rId79"/>
-    <hyperlink ref="H31" r:id="rId80"/>
-    <hyperlink ref="A32" r:id="rId81"/>
-    <hyperlink ref="G32" r:id="rId82"/>
-    <hyperlink ref="H32" r:id="rId83"/>
-    <hyperlink ref="A33" r:id="rId84"/>
-    <hyperlink ref="G33" r:id="rId85"/>
-    <hyperlink ref="H33" r:id="rId86"/>
-    <hyperlink ref="A34" r:id="rId87"/>
-    <hyperlink ref="G34" r:id="rId88"/>
-    <hyperlink ref="H34" r:id="rId89"/>
-    <hyperlink ref="A35" r:id="rId90"/>
-    <hyperlink ref="G35" r:id="rId91"/>
-    <hyperlink ref="H35" r:id="rId92"/>
-    <hyperlink ref="A36" r:id="rId93"/>
-    <hyperlink ref="G36" r:id="rId94"/>
-    <hyperlink ref="H36" r:id="rId95"/>
-    <hyperlink ref="A37" r:id="rId96"/>
-    <hyperlink ref="G37" r:id="rId97"/>
-    <hyperlink ref="H37" r:id="rId98"/>
-    <hyperlink ref="A38" r:id="rId99"/>
-    <hyperlink ref="G38" r:id="rId100"/>
-    <hyperlink ref="H38" r:id="rId101"/>
-    <hyperlink ref="A39" r:id="rId102"/>
-    <hyperlink ref="G39" r:id="rId103"/>
+    <hyperlink ref="A3" r:id="rId3" display="Scatch Jr by MIT"/>
+    <hyperlink ref="G3" r:id="rId4"/>
+    <hyperlink ref="A4" r:id="rId5"/>
+    <hyperlink ref="G4" r:id="rId6"/>
+    <hyperlink ref="G5" r:id="rId7"/>
+    <hyperlink ref="A6" r:id="rId8"/>
+    <hyperlink ref="G6" r:id="rId9"/>
+    <hyperlink ref="A7" r:id="rId10"/>
+    <hyperlink ref="G7" r:id="rId11"/>
+    <hyperlink ref="G8" r:id="rId12"/>
+    <hyperlink ref="A9" r:id="rId13"/>
+    <hyperlink ref="G9" r:id="rId14"/>
+    <hyperlink ref="A10" r:id="rId15"/>
+    <hyperlink ref="G10" r:id="rId16"/>
+    <hyperlink ref="A11" r:id="rId17"/>
+    <hyperlink ref="G11" r:id="rId18"/>
+    <hyperlink ref="A12" r:id="rId19"/>
+    <hyperlink ref="G12" r:id="rId20"/>
+    <hyperlink ref="A13" r:id="rId21"/>
+    <hyperlink ref="G13" r:id="rId22"/>
+    <hyperlink ref="A14" r:id="rId23"/>
+    <hyperlink ref="G14" r:id="rId24"/>
+    <hyperlink ref="A15" r:id="rId25" location="/"/>
+    <hyperlink ref="G15" r:id="rId26" location="/"/>
+    <hyperlink ref="A16" r:id="rId27"/>
+    <hyperlink ref="G16" r:id="rId28"/>
+    <hyperlink ref="A17" r:id="rId29" location="/user/GlowScriptDemos/folder/Examples/"/>
+    <hyperlink ref="G17" r:id="rId30" location="/user/GlowScriptDemos/folder/Examples/"/>
+    <hyperlink ref="A18" r:id="rId31"/>
+    <hyperlink ref="G18" r:id="rId32"/>
+    <hyperlink ref="A19" r:id="rId33"/>
+    <hyperlink ref="G19" r:id="rId34"/>
+    <hyperlink ref="A20" r:id="rId35"/>
+    <hyperlink ref="G20" r:id="rId36"/>
+    <hyperlink ref="A21" r:id="rId37"/>
+    <hyperlink ref="G21" r:id="rId38"/>
+    <hyperlink ref="A22" r:id="rId39"/>
+    <hyperlink ref="G22" r:id="rId40"/>
+    <hyperlink ref="A23" r:id="rId41"/>
+    <hyperlink ref="G23" r:id="rId42"/>
+    <hyperlink ref="A24" r:id="rId43"/>
+    <hyperlink ref="G24" r:id="rId44"/>
+    <hyperlink ref="A25" r:id="rId45"/>
+    <hyperlink ref="G25" r:id="rId46"/>
+    <hyperlink ref="A26" r:id="rId47"/>
+    <hyperlink ref="G26" r:id="rId48"/>
+    <hyperlink ref="A27" r:id="rId49"/>
+    <hyperlink ref="G27" r:id="rId50"/>
+    <hyperlink ref="A28" r:id="rId51"/>
+    <hyperlink ref="G28" r:id="rId52"/>
+    <hyperlink ref="A29" r:id="rId53"/>
+    <hyperlink ref="G29" r:id="rId54"/>
+    <hyperlink ref="A30" r:id="rId55"/>
+    <hyperlink ref="G30" r:id="rId56"/>
+    <hyperlink ref="A31" r:id="rId57"/>
+    <hyperlink ref="G31" r:id="rId58"/>
+    <hyperlink ref="A32" r:id="rId59"/>
+    <hyperlink ref="G32" r:id="rId60"/>
+    <hyperlink ref="A33" r:id="rId61"/>
+    <hyperlink ref="G33" r:id="rId62"/>
+    <hyperlink ref="A34" r:id="rId63"/>
+    <hyperlink ref="G34" r:id="rId64"/>
+    <hyperlink ref="A35" r:id="rId65"/>
+    <hyperlink ref="G35" r:id="rId66"/>
+    <hyperlink ref="A36" r:id="rId67"/>
+    <hyperlink ref="G36" r:id="rId68"/>
+    <hyperlink ref="A37" r:id="rId69"/>
+    <hyperlink ref="G37" r:id="rId70"/>
+    <hyperlink ref="A38" r:id="rId71"/>
+    <hyperlink ref="G38" r:id="rId72"/>
+    <hyperlink ref="A39" r:id="rId73"/>
+    <hyperlink ref="G39" r:id="rId74"/>
+    <hyperlink ref="H16" r:id="rId75"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -15426,17 +15461,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="14">
-      <c r="A1" s="40" t="s">
+      <c r="A1" s="41" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="41"/>
+      <c r="B1" s="42"/>
     </row>
     <row r="2" spans="1:2" ht="14">
-      <c r="A2" s="42"/>
-      <c r="B2" s="43"/>
+      <c r="A2" s="43"/>
+      <c r="B2" s="44"/>
     </row>
     <row r="3" spans="1:2" ht="14">
-      <c r="A3" s="44" t="s">
+      <c r="A3" s="45" t="s">
         <v>10</v>
       </c>
       <c r="B3" s="4" t="s">
@@ -15444,37 +15479,37 @@
       </c>
     </row>
     <row r="4" spans="1:2" ht="14">
-      <c r="A4" s="45"/>
+      <c r="A4" s="46"/>
       <c r="B4" s="4" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="14">
-      <c r="A5" s="45"/>
+      <c r="A5" s="46"/>
       <c r="B5" s="4" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="14">
-      <c r="A6" s="45"/>
+      <c r="A6" s="46"/>
       <c r="B6" s="4" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="14">
-      <c r="A7" s="45"/>
+      <c r="A7" s="46"/>
       <c r="B7" s="4" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="14">
-      <c r="A8" s="45"/>
+      <c r="A8" s="46"/>
       <c r="B8" s="6" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="14">
-      <c r="A9" s="44" t="s">
+      <c r="A9" s="45" t="s">
         <v>3</v>
       </c>
       <c r="B9" s="4" t="s">
@@ -15482,239 +15517,239 @@
       </c>
     </row>
     <row r="10" spans="1:2" ht="14">
-      <c r="A10" s="45"/>
+      <c r="A10" s="46"/>
       <c r="B10" s="4" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="14">
-      <c r="A11" s="45"/>
+      <c r="A11" s="46"/>
       <c r="B11" s="4" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="14">
-      <c r="A12" s="45"/>
+      <c r="A12" s="46"/>
       <c r="B12" s="4" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="14">
-      <c r="A13" s="45"/>
+      <c r="A13" s="46"/>
       <c r="B13" s="4" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="14" spans="1:2" ht="14">
-      <c r="A14" s="45"/>
+      <c r="A14" s="46"/>
       <c r="B14" s="4" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="15" spans="1:2" ht="14">
-      <c r="A15" s="45"/>
+      <c r="A15" s="46"/>
       <c r="B15" s="4" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="16" spans="1:2" ht="14">
-      <c r="A16" s="45"/>
+      <c r="A16" s="46"/>
       <c r="B16" s="4" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="14">
-      <c r="A17" s="45"/>
+      <c r="A17" s="46"/>
       <c r="B17" s="4" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="14">
-      <c r="A18" s="45"/>
+      <c r="A18" s="46"/>
       <c r="B18" s="4" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" ht="14">
+      <c r="A19" s="46"/>
+      <c r="B19" s="9" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="19" spans="1:2" ht="14">
-      <c r="A19" s="45"/>
-      <c r="B19" s="9" t="s">
-        <v>34</v>
-      </c>
-    </row>
     <row r="20" spans="1:2" ht="14">
-      <c r="A20" s="46"/>
+      <c r="A20" s="47"/>
       <c r="B20" s="10" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="21" spans="1:2" ht="15.75" customHeight="1">
-      <c r="A21" s="47" t="s">
+      <c r="A21" s="48" t="s">
         <v>9</v>
       </c>
       <c r="B21" s="9" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" ht="15.75" customHeight="1">
+      <c r="A22" s="46"/>
+      <c r="B22" s="4" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="22" spans="1:2" ht="15.75" customHeight="1">
-      <c r="A22" s="45"/>
-      <c r="B22" s="4" t="s">
+    <row r="23" spans="1:2" ht="15.75" customHeight="1">
+      <c r="A23" s="46"/>
+      <c r="B23" s="4" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="23" spans="1:2" ht="15.75" customHeight="1">
-      <c r="A23" s="45"/>
-      <c r="B23" s="4" t="s">
+    <row r="24" spans="1:2" ht="15.75" customHeight="1">
+      <c r="A24" s="46"/>
+      <c r="B24" s="4" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="24" spans="1:2" ht="15.75" customHeight="1">
-      <c r="A24" s="45"/>
-      <c r="B24" s="4" t="s">
+    <row r="25" spans="1:2" ht="15.75" customHeight="1">
+      <c r="A25" s="46"/>
+      <c r="B25" s="4" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="25" spans="1:2" ht="15.75" customHeight="1">
-      <c r="A25" s="45"/>
-      <c r="B25" s="4" t="s">
+    <row r="26" spans="1:2" ht="15.75" customHeight="1">
+      <c r="A26" s="46"/>
+      <c r="B26" s="4" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="26" spans="1:2" ht="15.75" customHeight="1">
-      <c r="A26" s="45"/>
-      <c r="B26" s="4" t="s">
+    <row r="27" spans="1:2" ht="15.75" customHeight="1">
+      <c r="A27" s="46"/>
+      <c r="B27" s="4" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="27" spans="1:2" ht="15.75" customHeight="1">
-      <c r="A27" s="45"/>
-      <c r="B27" s="4" t="s">
-        <v>42</v>
-      </c>
-    </row>
     <row r="28" spans="1:2" ht="15.75" customHeight="1">
-      <c r="A28" s="45"/>
+      <c r="A28" s="46"/>
       <c r="B28" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="29" spans="1:2" ht="15.75" customHeight="1">
-      <c r="A29" s="45"/>
+      <c r="A29" s="46"/>
       <c r="B29" s="4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="30" spans="1:2" ht="15.75" customHeight="1">
-      <c r="A30" s="45"/>
+      <c r="A30" s="46"/>
       <c r="B30" s="4" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" ht="15.75" customHeight="1">
+      <c r="A31" s="46"/>
+      <c r="B31" s="4" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="31" spans="1:2" ht="15.75" customHeight="1">
-      <c r="A31" s="45"/>
-      <c r="B31" s="4" t="s">
+    <row r="32" spans="1:2" ht="15.75" customHeight="1">
+      <c r="A32" s="46"/>
+      <c r="B32" s="4" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="32" spans="1:2" ht="15.75" customHeight="1">
-      <c r="A32" s="45"/>
-      <c r="B32" s="4" t="s">
+    <row r="33" spans="1:2" ht="15.75" customHeight="1">
+      <c r="A33" s="46"/>
+      <c r="B33" s="4" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="33" spans="1:2" ht="15.75" customHeight="1">
-      <c r="A33" s="45"/>
-      <c r="B33" s="4" t="s">
+    <row r="34" spans="1:2" ht="15.75" customHeight="1">
+      <c r="A34" s="46"/>
+      <c r="B34" s="9" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="34" spans="1:2" ht="15.75" customHeight="1">
-      <c r="A34" s="45"/>
-      <c r="B34" s="9" t="s">
+    <row r="35" spans="1:2" ht="15.75" customHeight="1">
+      <c r="A35" s="46"/>
+      <c r="B35" s="4" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="35" spans="1:2" ht="15.75" customHeight="1">
-      <c r="A35" s="45"/>
-      <c r="B35" s="4" t="s">
+    <row r="36" spans="1:2" ht="15.75" customHeight="1">
+      <c r="A36" s="46"/>
+      <c r="B36" s="4" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="36" spans="1:2" ht="15.75" customHeight="1">
-      <c r="A36" s="45"/>
-      <c r="B36" s="4" t="s">
+    <row r="37" spans="1:2" ht="15.75" customHeight="1">
+      <c r="A37" s="46"/>
+      <c r="B37" s="4" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="37" spans="1:2" ht="15.75" customHeight="1">
-      <c r="A37" s="45"/>
-      <c r="B37" s="4" t="s">
+    <row r="38" spans="1:2" ht="15.75" customHeight="1">
+      <c r="A38" s="46"/>
+      <c r="B38" s="4" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="38" spans="1:2" ht="15.75" customHeight="1">
-      <c r="A38" s="45"/>
-      <c r="B38" s="4" t="s">
-        <v>58</v>
-      </c>
-    </row>
     <row r="39" spans="1:2" ht="15.75" customHeight="1">
-      <c r="A39" s="45"/>
+      <c r="A39" s="46"/>
       <c r="B39" s="6" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="40" spans="1:2" ht="15.75" customHeight="1">
-      <c r="A40" s="45"/>
+      <c r="A40" s="46"/>
       <c r="B40" s="13" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="41" spans="1:2" ht="15.75" customHeight="1">
-      <c r="A41" s="44" t="s">
+      <c r="A41" s="45" t="s">
+        <v>59</v>
+      </c>
+      <c r="B41" s="4" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" ht="15.75" customHeight="1">
+      <c r="A42" s="46"/>
+      <c r="B42" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="B41" s="4" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="42" spans="1:2" ht="15.75" customHeight="1">
-      <c r="A42" s="45"/>
-      <c r="B42" s="4" t="s">
+    </row>
+    <row r="43" spans="1:2" ht="15.75" customHeight="1">
+      <c r="A43" s="46"/>
+      <c r="B43" s="4" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" ht="15.75" customHeight="1">
+      <c r="A44" s="46"/>
+      <c r="B44" s="4" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="43" spans="1:2" ht="15.75" customHeight="1">
-      <c r="A43" s="45"/>
-      <c r="B43" s="4" t="s">
+    <row r="45" spans="1:2" ht="15.75" customHeight="1">
+      <c r="A45" s="46"/>
+      <c r="B45" s="4" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="44" spans="1:2" ht="15.75" customHeight="1">
-      <c r="A44" s="45"/>
-      <c r="B44" s="4" t="s">
+    <row r="46" spans="1:2" ht="15.75" customHeight="1">
+      <c r="A46" s="46"/>
+      <c r="B46" s="4" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="45" spans="1:2" ht="15.75" customHeight="1">
-      <c r="A45" s="45"/>
-      <c r="B45" s="4" t="s">
+    <row r="47" spans="1:2" ht="15.75" customHeight="1">
+      <c r="A47" s="46"/>
+      <c r="B47" s="4" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="46" spans="1:2" ht="15.75" customHeight="1">
-      <c r="A46" s="45"/>
-      <c r="B46" s="4" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="47" spans="1:2" ht="15.75" customHeight="1">
-      <c r="A47" s="45"/>
-      <c r="B47" s="4" t="s">
-        <v>68</v>
-      </c>
-    </row>
     <row r="48" spans="1:2" ht="15.75" customHeight="1">
-      <c r="A48" s="46"/>
+      <c r="A48" s="47"/>
       <c r="B48" s="10" t="s">
         <v>16</v>
       </c>
@@ -15724,75 +15759,75 @@
         <v>6</v>
       </c>
       <c r="B49" s="15" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" ht="15.75" customHeight="1">
+      <c r="A50" s="38" t="s">
+        <v>72</v>
+      </c>
+      <c r="B50" s="8" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="50" spans="1:2" ht="15.75" customHeight="1">
-      <c r="A50" s="37" t="s">
-        <v>75</v>
-      </c>
-      <c r="B50" s="8" t="s">
-        <v>76</v>
-      </c>
-    </row>
     <row r="51" spans="1:2" ht="15.75" customHeight="1">
-      <c r="A51" s="38"/>
+      <c r="A51" s="39"/>
       <c r="B51" s="8" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" ht="15.75" customHeight="1">
+      <c r="A52" s="39"/>
+      <c r="B52" s="8" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" ht="15.75" customHeight="1">
+      <c r="A53" s="39"/>
+      <c r="B53" s="8" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" ht="15.75" customHeight="1">
+      <c r="A54" s="39"/>
+      <c r="B54" s="8" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="52" spans="1:2" ht="15.75" customHeight="1">
-      <c r="A52" s="38"/>
-      <c r="B52" s="8" t="s">
+    <row r="55" spans="1:2" ht="15.75" customHeight="1">
+      <c r="A55" s="39"/>
+      <c r="B55" s="8" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="53" spans="1:2" ht="15.75" customHeight="1">
-      <c r="A53" s="38"/>
-      <c r="B53" s="8" t="s">
+    <row r="56" spans="1:2" ht="15.75" customHeight="1">
+      <c r="A56" s="39"/>
+      <c r="B56" s="8" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="54" spans="1:2" ht="15.75" customHeight="1">
-      <c r="A54" s="38"/>
-      <c r="B54" s="8" t="s">
+    <row r="57" spans="1:2" ht="15.75" customHeight="1">
+      <c r="A57" s="39"/>
+      <c r="B57" s="8" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="55" spans="1:2" ht="15.75" customHeight="1">
-      <c r="A55" s="38"/>
-      <c r="B55" s="8" t="s">
+    <row r="58" spans="1:2" ht="15.75" customHeight="1">
+      <c r="A58" s="39"/>
+      <c r="B58" s="8" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="56" spans="1:2" ht="15.75" customHeight="1">
-      <c r="A56" s="38"/>
-      <c r="B56" s="8" t="s">
+    <row r="59" spans="1:2" ht="15.75" customHeight="1">
+      <c r="A59" s="39"/>
+      <c r="B59" s="16" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="57" spans="1:2" ht="15.75" customHeight="1">
-      <c r="A57" s="38"/>
-      <c r="B57" s="8" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="58" spans="1:2" ht="15.75" customHeight="1">
-      <c r="A58" s="38"/>
-      <c r="B58" s="8" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="59" spans="1:2" ht="15.75" customHeight="1">
-      <c r="A59" s="38"/>
-      <c r="B59" s="16" t="s">
-        <v>92</v>
-      </c>
-    </row>
     <row r="60" spans="1:2" ht="15.75" customHeight="1">
-      <c r="A60" s="39"/>
+      <c r="A60" s="40"/>
       <c r="B60" s="13" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
     </row>
     <row r="61" spans="1:2" ht="15.75" customHeight="1"/>

</xml_diff>